<commit_message>
trying to run a bunch of rays
</commit_message>
<xml_diff>
--- a/example_scripts/more_conjunctions.xlsx
+++ b/example_scripts/more_conjunctions.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rileyannereid/PycharmProjects/Stanford_Raytracer/example_scripts/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91917861-4C3B-2743-867B-7CBB2AADB8CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,6 +58,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -98,7 +112,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -130,9 +144,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -164,6 +196,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -339,31 +389,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:N127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>-0.8171731384121697</v>
+        <v>-0.81717313841216965</v>
       </c>
       <c r="B2">
-        <v>2.044887635466501</v>
+        <v>2.0448876354665009</v>
       </c>
       <c r="C2">
-        <v>-0.5503398103054989</v>
+        <v>-0.55033981030549894</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="F2">
-        <v>1.568953591805656</v>
+        <v>1.5689535918056561</v>
       </c>
       <c r="G2">
-        <v>-0.4025301319793025</v>
+        <v>-0.40253013197930249</v>
       </c>
       <c r="H2">
         <v>1.259052189153208</v>
@@ -372,10 +422,10 @@
         <v>1</v>
       </c>
       <c r="K2">
-        <v>-0.6654032015642056</v>
+        <v>-0.66540320156420563</v>
       </c>
       <c r="L2">
-        <v>-2.551178041985491</v>
+        <v>-2.5511780419854908</v>
       </c>
       <c r="M2">
         <v>-1.094989555154213</v>
@@ -384,97 +434,97 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>-0.818688240068262</v>
+        <v>-0.81868824006826202</v>
       </c>
       <c r="B3">
-        <v>2.049245743741911</v>
+        <v>2.0492457437419112</v>
       </c>
       <c r="C3">
-        <v>-0.5463670061579023</v>
+        <v>-0.54636700615790235</v>
       </c>
       <c r="D3">
-        <v>0.9975132690579486</v>
+        <v>0.99751326905794857</v>
       </c>
       <c r="F3">
-        <v>1.56048946534531</v>
+        <v>1.5604894653453101</v>
       </c>
       <c r="G3">
-        <v>-0.4008786614777741</v>
+        <v>-0.40087866147777412</v>
       </c>
       <c r="H3">
-        <v>1.258367947990407</v>
+        <v>1.2583679479904071</v>
       </c>
       <c r="I3">
         <v>1.005658903714671</v>
       </c>
       <c r="K3">
-        <v>-0.6658264264660786</v>
+        <v>-0.66582642646607859</v>
       </c>
       <c r="L3">
-        <v>-2.55372003874137</v>
+        <v>-2.5537200387413699</v>
       </c>
       <c r="M3">
         <v>-1.093131689169007</v>
       </c>
       <c r="N3">
-        <v>0.9991720368565292</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+        <v>0.99917203685652922</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>-0.8201960383607291</v>
+        <v>-0.82019603836072907</v>
       </c>
       <c r="B4">
-        <v>2.05358325838859</v>
+        <v>2.0535832583885898</v>
       </c>
       <c r="C4">
-        <v>-0.5423979689442681</v>
+        <v>-0.54239796894426806</v>
       </c>
       <c r="D4">
-        <v>0.9950494094356566</v>
+        <v>0.99504940943565656</v>
       </c>
       <c r="F4">
-        <v>1.55197137105583</v>
+        <v>1.5519713710558301</v>
       </c>
       <c r="G4">
-        <v>-0.3992104629187047</v>
+        <v>-0.39921046291870471</v>
       </c>
       <c r="H4">
         <v>1.257644673885985</v>
       </c>
       <c r="I4">
-        <v>1.011417769775751</v>
+        <v>1.0114177697757509</v>
       </c>
       <c r="K4">
-        <v>-0.6662471024611872</v>
+        <v>-0.66624710246118724</v>
       </c>
       <c r="L4">
-        <v>-2.556253118736662</v>
+        <v>-2.5562531187366622</v>
       </c>
       <c r="M4">
         <v>-1.091274202221644</v>
       </c>
       <c r="N4">
-        <v>0.9983486808759801</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+        <v>0.99834868087598005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>-0.8220704610690257</v>
       </c>
       <c r="B5">
-        <v>2.058976050036397</v>
+        <v>2.0589760500363972</v>
       </c>
       <c r="C5">
-        <v>-0.5374423464226417</v>
+        <v>-0.53744234642264166</v>
       </c>
       <c r="D5">
-        <v>0.9920014754990772</v>
+        <v>0.99200147549907725</v>
       </c>
       <c r="F5">
-        <v>1.541247793054099</v>
+        <v>1.5412477930540991</v>
       </c>
       <c r="G5">
         <v>-0.3971014057502858</v>
@@ -486,74 +536,74 @@
         <v>1.018760492499013</v>
       </c>
       <c r="K5">
-        <v>-0.666769377599817</v>
+        <v>-0.66676937759981703</v>
       </c>
       <c r="L5">
-        <v>-2.559407006469969</v>
+        <v>-2.5594070064699692</v>
       </c>
       <c r="M5">
-        <v>-1.088952838845271</v>
+        <v>-1.0889528388452709</v>
       </c>
       <c r="N5">
-        <v>0.9973258994882456</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+        <v>0.99732589948824557</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>-0.8243974690385852</v>
+        <v>-0.82439746903858524</v>
       </c>
       <c r="B6">
         <v>2.065671805492256</v>
       </c>
       <c r="C6">
-        <v>-0.5312569190362165</v>
+        <v>-0.53125691903621652</v>
       </c>
       <c r="D6">
-        <v>0.9882406041884612</v>
+        <v>0.98824060418846116</v>
       </c>
       <c r="F6">
-        <v>1.530438186496783</v>
+        <v>1.5304381864967831</v>
       </c>
       <c r="G6">
-        <v>-0.3949649536739925</v>
+        <v>-0.39496495367399248</v>
       </c>
       <c r="H6">
-        <v>1.25565947610929</v>
+        <v>1.2556594761092901</v>
       </c>
       <c r="I6">
         <v>1.026268905272895</v>
       </c>
       <c r="K6">
-        <v>-0.6674166622356101</v>
+        <v>-0.66741666223561014</v>
       </c>
       <c r="L6">
-        <v>-2.563329871124924</v>
+        <v>-2.5633298711249242</v>
       </c>
       <c r="M6">
-        <v>-1.086051962636117</v>
+        <v>-1.0860519626361169</v>
       </c>
       <c r="N6">
-        <v>0.9960573920492006</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+        <v>0.99605739204920063</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>-0.8272813801361592</v>
+        <v>-0.82728138013615915</v>
       </c>
       <c r="B7">
-        <v>2.073971236017589</v>
+        <v>2.0739712360175888</v>
       </c>
       <c r="C7">
-        <v>-0.5235398509066876</v>
+        <v>-0.52353985090668764</v>
       </c>
       <c r="D7">
-        <v>0.983614685226346</v>
+        <v>0.98361468522634599</v>
       </c>
       <c r="F7">
-        <v>1.516806349315272</v>
+        <v>1.5168063493152719</v>
       </c>
       <c r="G7">
-        <v>-0.3922552380296158</v>
+        <v>-0.39225523802961582</v>
       </c>
       <c r="H7">
         <v>1.254285203305183</v>
@@ -562,45 +612,45 @@
         <v>1.03589413704902</v>
       </c>
       <c r="K7">
-        <v>-0.6682171352274349</v>
+        <v>-0.66821713522743487</v>
       </c>
       <c r="L7">
-        <v>-2.568203130423557</v>
+        <v>-2.5682031304235569</v>
       </c>
       <c r="M7">
         <v>-1.082427104646783</v>
       </c>
       <c r="N7">
-        <v>0.9944871775592892</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+        <v>0.99448717755928917</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>-0.830847866606804</v>
+        <v>-0.83084786660680399</v>
       </c>
       <c r="B8">
         <v>2.084236734309957</v>
       </c>
       <c r="C8">
-        <v>-0.5139170481390217</v>
+        <v>-0.51391704813902173</v>
       </c>
       <c r="D8">
-        <v>0.9779468379145578</v>
+        <v>0.97794683791455783</v>
       </c>
       <c r="F8">
         <v>1.499571544035609</v>
       </c>
       <c r="G8">
-        <v>-0.3888053556617777</v>
+        <v>-0.38880535566177771</v>
       </c>
       <c r="H8">
-        <v>1.252415059546533</v>
+        <v>1.2524150595465331</v>
       </c>
       <c r="I8">
         <v>1.04832017218639</v>
       </c>
       <c r="K8">
-        <v>-0.6692042399655589</v>
+        <v>-0.66920423996555889</v>
       </c>
       <c r="L8">
         <v>-2.574247207756811</v>
@@ -609,65 +659,65 @@
         <v>-1.077898150977503</v>
       </c>
       <c r="N8">
-        <v>0.9925483287965468</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+        <v>0.99254832879654675</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>-0.8352460523428039</v>
+        <v>-0.83524605234280391</v>
       </c>
       <c r="B9">
-        <v>2.096898397824664</v>
+        <v>2.0968983978246638</v>
       </c>
       <c r="C9">
-        <v>-0.5019281719831962</v>
+        <v>-0.50192817198319617</v>
       </c>
       <c r="D9">
-        <v>0.9710367034745476</v>
+        <v>0.97103670347454762</v>
       </c>
       <c r="F9">
-        <v>1.482120023712843</v>
+        <v>1.4821200237128429</v>
       </c>
       <c r="G9">
-        <v>-0.3852837518440876</v>
+        <v>-0.38528375184408759</v>
       </c>
       <c r="H9">
         <v>1.250368054108969</v>
       </c>
       <c r="I9">
-        <v>1.061204387249082</v>
+        <v>1.0612043872490819</v>
       </c>
       <c r="K9">
-        <v>-0.6704172688912807</v>
+        <v>-0.67041726889128073</v>
       </c>
       <c r="L9">
-        <v>-2.581728778272265</v>
+        <v>-2.5817287782722649</v>
       </c>
       <c r="M9">
-        <v>-1.07223996677095</v>
+        <v>-1.0722399667709499</v>
       </c>
       <c r="N9">
-        <v>0.9901615077917648</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+        <v>0.99016150779176482</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>-0.8406508554844286</v>
+        <v>-0.84065085548442864</v>
       </c>
       <c r="B10">
-        <v>2.112461310179648</v>
+        <v>2.1124613101796479</v>
       </c>
       <c r="C10">
-        <v>-0.4870070521853599</v>
+        <v>-0.48700705218535989</v>
       </c>
       <c r="D10">
-        <v>0.9626627117200977</v>
+        <v>0.96266271172009765</v>
       </c>
       <c r="F10">
         <v>1.459987636435325</v>
       </c>
       <c r="G10">
-        <v>-0.380774500734367</v>
+        <v>-0.38077450073436703</v>
       </c>
       <c r="H10">
         <v>1.247546165148806</v>
@@ -676,74 +726,74 @@
         <v>1.077998794449339</v>
       </c>
       <c r="K10">
-        <v>-0.6719013482784992</v>
+        <v>-0.67190134827849923</v>
       </c>
       <c r="L10">
-        <v>-2.590967090773522</v>
+        <v>-2.5909670907735221</v>
       </c>
       <c r="M10">
         <v>-1.065171453025183</v>
       </c>
       <c r="N10">
-        <v>0.987234209204476</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+        <v>0.98723420920447602</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>-0.8472645532676997</v>
+        <v>-0.84726455326769967</v>
       </c>
       <c r="B11">
         <v>2.131509877426915</v>
       </c>
       <c r="C11">
-        <v>-0.4684581006684945</v>
+        <v>-0.46845810066849453</v>
       </c>
       <c r="D11">
-        <v>0.952587803908824</v>
+        <v>0.95258780390882403</v>
       </c>
       <c r="F11">
-        <v>1.437499544378719</v>
+        <v>1.4374995443787191</v>
       </c>
       <c r="G11">
-        <v>-0.3761432612581807</v>
+        <v>-0.37614326125818071</v>
       </c>
       <c r="H11">
-        <v>1.244414224284547</v>
+        <v>1.2444142242845471</v>
       </c>
       <c r="I11">
-        <v>1.095606226603025</v>
+        <v>1.0956062266030251</v>
       </c>
       <c r="K11">
-        <v>-0.6737065086675265</v>
+        <v>-0.67370650866752646</v>
       </c>
       <c r="L11">
-        <v>-2.602337212102406</v>
+        <v>-2.6023372121024062</v>
       </c>
       <c r="M11">
-        <v>-1.056343566776459</v>
+        <v>-1.0563435667764589</v>
       </c>
       <c r="N11">
-        <v>0.9836615089423512</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+        <v>0.98366150894235116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>-0.8537204688592824</v>
+        <v>-0.85372046885928243</v>
       </c>
       <c r="B12">
-        <v>2.15010884278205</v>
+        <v>2.1501088427820498</v>
       </c>
       <c r="C12">
-        <v>-0.4500310008942588</v>
+        <v>-0.45003100089425879</v>
       </c>
       <c r="D12">
-        <v>0.9429304618934132</v>
+        <v>0.94293046189341323</v>
       </c>
       <c r="F12">
         <v>1.408869866184064</v>
       </c>
       <c r="G12">
-        <v>-0.3701737802171151</v>
+        <v>-0.37017378021711511</v>
       </c>
       <c r="H12">
         <v>1.240030006544703</v>
@@ -752,27 +802,27 @@
         <v>1.118856088485656</v>
       </c>
       <c r="K12">
-        <v>-0.6758860387392022</v>
+        <v>-0.67588603873920217</v>
       </c>
       <c r="L12">
-        <v>-2.616275359352023</v>
+        <v>-2.6162753593520232</v>
       </c>
       <c r="M12">
-        <v>-1.045320000783662</v>
+        <v>-1.0453200007836621</v>
       </c>
       <c r="N12">
-        <v>0.9793268754907896</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+        <v>0.97932687549078956</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>-0.8600208254473861</v>
+        <v>-0.86002082544738612</v>
       </c>
       <c r="B13">
-        <v>2.168262990350062</v>
+        <v>2.1682629903500619</v>
       </c>
       <c r="C13">
-        <v>-0.4317284497925143</v>
+        <v>-0.43172844979251429</v>
       </c>
       <c r="D13">
         <v>0.933669710265292</v>
@@ -784,42 +834,42 @@
         <v>-0.3639916900261212</v>
       </c>
       <c r="H13">
-        <v>1.235083467729242</v>
+        <v>1.2350834677292419</v>
       </c>
       <c r="I13">
-        <v>1.143600030377646</v>
+        <v>1.1436000303776459</v>
       </c>
       <c r="K13">
-        <v>-0.678492637151809</v>
+        <v>-0.67849263715180896</v>
       </c>
       <c r="L13">
-        <v>-2.633274228685</v>
+        <v>-2.6332742286849999</v>
       </c>
       <c r="M13">
-        <v>-1.031557419054495</v>
+        <v>-1.0315574190544949</v>
       </c>
       <c r="N13">
-        <v>0.9741069010575464</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
+        <v>0.97410690105754638</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>-0.8676806552691642</v>
+        <v>-0.86768065526916416</v>
       </c>
       <c r="B14">
-        <v>2.190338183907118</v>
+        <v>2.1903381839071181</v>
       </c>
       <c r="C14">
-        <v>-0.409026716432101</v>
+        <v>-0.40902671643210098</v>
       </c>
       <c r="D14">
-        <v>0.9226213776056856</v>
+        <v>0.92262137760568563</v>
       </c>
       <c r="F14">
         <v>1.349842006578978</v>
       </c>
       <c r="G14">
-        <v>-0.3575839694509221</v>
+        <v>-0.35758396945092208</v>
       </c>
       <c r="H14">
         <v>1.229523931511908</v>
@@ -828,74 +878,74 @@
         <v>1.16998451227703</v>
       </c>
       <c r="K14">
-        <v>-0.6815705348594703</v>
+        <v>-0.68157053485947028</v>
       </c>
       <c r="L14">
-        <v>-2.653869132463354</v>
+        <v>-2.6538691324633539</v>
       </c>
       <c r="M14">
-        <v>-1.014380595744865</v>
+        <v>-1.0143805957448651</v>
       </c>
       <c r="N14">
-        <v>0.9678797565013186</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+        <v>0.96787975650131863</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>-0.8769216438924384</v>
+        <v>-0.87692164389243843</v>
       </c>
       <c r="B15">
-        <v>2.216976763331257</v>
+        <v>2.2169767633312571</v>
       </c>
       <c r="C15">
-        <v>-0.3809293701982359</v>
+        <v>-0.38092937019823592</v>
       </c>
       <c r="D15">
-        <v>0.9095868583688096</v>
+        <v>0.90958685836880959</v>
       </c>
       <c r="F15">
         <v>1.319407827587497</v>
       </c>
       <c r="G15">
-        <v>-0.3509350041999207</v>
+        <v>-0.35093500419992069</v>
       </c>
       <c r="H15">
-        <v>1.223293795246568</v>
+        <v>1.2232937952465679</v>
       </c>
       <c r="I15">
-        <v>1.198177926560514</v>
+        <v>1.1981779265605139</v>
       </c>
       <c r="K15">
-        <v>-0.6844536635565444</v>
+        <v>-0.68445366355654436</v>
       </c>
       <c r="L15">
         <v>-2.673751668093534</v>
       </c>
       <c r="M15">
-        <v>-0.9972306715786773</v>
+        <v>-0.99723067157867729</v>
       </c>
       <c r="N15">
-        <v>0.9619688662190322</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+        <v>0.96196886621903221</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>-0.887958464018157</v>
+        <v>-0.88795846401815703</v>
       </c>
       <c r="B16">
-        <v>2.248807037179199</v>
+        <v>2.2488070371791991</v>
       </c>
       <c r="C16">
-        <v>-0.3462427406519591</v>
+        <v>-0.34624274065195909</v>
       </c>
       <c r="D16">
-        <v>0.8944168435208357</v>
+        <v>0.89441684352083572</v>
       </c>
       <c r="F16">
         <v>1.288353322492702</v>
       </c>
       <c r="G16">
-        <v>-0.3440348090918571</v>
+        <v>-0.34403480909185707</v>
       </c>
       <c r="H16">
         <v>1.216332106192431</v>
@@ -907,65 +957,65 @@
         <v>-0.68714750869579</v>
       </c>
       <c r="L16">
-        <v>-2.692936073745854</v>
+        <v>-2.6929360737458539</v>
       </c>
       <c r="M16">
-        <v>-0.9801052876943683</v>
+        <v>-0.98010528769436833</v>
       </c>
       <c r="N16">
-        <v>0.9563590127034139</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
+        <v>0.95635901270341395</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>-0.8984339731085174</v>
+        <v>-0.89843397310851736</v>
       </c>
       <c r="B17">
-        <v>2.27903539610714</v>
+        <v>2.2790353961071399</v>
       </c>
       <c r="C17">
-        <v>-0.3120306596386558</v>
+        <v>-0.31203065963865578</v>
       </c>
       <c r="D17">
-        <v>0.8803932553792246</v>
+        <v>0.88039325537922464</v>
       </c>
       <c r="F17">
         <v>1.256658320432354</v>
       </c>
       <c r="G17">
-        <v>-0.3368644230882942</v>
+        <v>-0.33686442308829417</v>
       </c>
       <c r="H17">
         <v>1.208565560180751</v>
       </c>
       <c r="I17">
-        <v>1.260722501529837</v>
+        <v>1.2607225015298369</v>
       </c>
       <c r="K17">
-        <v>-0.6896571603505113</v>
+        <v>-0.68965716035051128</v>
       </c>
       <c r="L17">
         <v>-2.711433579348475</v>
       </c>
       <c r="M17">
-        <v>-0.9630051334648499</v>
+        <v>-0.96300513346484995</v>
       </c>
       <c r="N17">
-        <v>0.9510367583500264</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
+        <v>0.95103675835002643</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>-0.9083576362221646</v>
+        <v>-0.90835763622216459</v>
       </c>
       <c r="B18">
-        <v>2.307688520861866</v>
+        <v>2.3076885208618658</v>
       </c>
       <c r="C18">
-        <v>-0.2782858704157288</v>
+        <v>-0.27828587041572878</v>
       </c>
       <c r="D18">
-        <v>0.8674211696551252</v>
+        <v>0.86742116965512517</v>
       </c>
       <c r="F18">
         <v>1.224341046062672</v>
@@ -974,7 +1024,7 @@
         <v>-0.3294100774282136</v>
       </c>
       <c r="H18">
-        <v>1.199921398598916</v>
+        <v>1.1999213985989159</v>
       </c>
       <c r="I18">
         <v>1.295493867870497</v>
@@ -986,97 +1036,97 @@
         <v>-2.729253299093946</v>
       </c>
       <c r="M18">
-        <v>-0.9459334102543783</v>
+        <v>-0.94593341025437827</v>
       </c>
       <c r="N18">
-        <v>0.9459900946693552</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
+        <v>0.94599009466935524</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>-0.9177433681000375</v>
+        <v>-0.91774336810003754</v>
       </c>
       <c r="B19">
         <v>2.334815098886335</v>
       </c>
       <c r="C19">
-        <v>-0.2449754043589459</v>
+        <v>-0.24497540435894591</v>
       </c>
       <c r="D19">
-        <v>0.8554072748927815</v>
+        <v>0.85540727489278146</v>
       </c>
       <c r="F19">
-        <v>1.191390524862891</v>
+        <v>1.1913905248628911</v>
       </c>
       <c r="G19">
-        <v>-0.321651657950653</v>
+        <v>-0.32165165795065298</v>
       </c>
       <c r="H19">
         <v>1.190308161675671</v>
       </c>
       <c r="I19">
-        <v>1.332931669089407</v>
+        <v>1.3329316690894071</v>
       </c>
       <c r="K19">
-        <v>-0.6941441552056964</v>
+        <v>-0.69414415520569639</v>
       </c>
       <c r="L19">
-        <v>-2.746415397696571</v>
+        <v>-2.7464153976965711</v>
       </c>
       <c r="M19">
-        <v>-0.9288815481991772</v>
+        <v>-0.92888154819917723</v>
       </c>
       <c r="N19">
-        <v>0.9412046429949767</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
+        <v>0.94120464299497675</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>-0.9287291390539797</v>
+        <v>-0.92872913905397969</v>
       </c>
       <c r="B20">
         <v>2.366613313325479</v>
       </c>
       <c r="C20">
-        <v>-0.2039437144765751</v>
+        <v>-0.20394371447657511</v>
       </c>
       <c r="D20">
-        <v>0.8416266108213668</v>
+        <v>0.84162661082136681</v>
       </c>
       <c r="F20">
         <v>1.15783271600237</v>
       </c>
       <c r="G20">
-        <v>-0.3135757457103809</v>
+        <v>-0.31357574571038088</v>
       </c>
       <c r="H20">
-        <v>1.179633426032494</v>
+        <v>1.1796334260324941</v>
       </c>
       <c r="I20">
         <v>1.37329547004607</v>
       </c>
       <c r="K20">
-        <v>-0.6966027385245905</v>
+        <v>-0.69660273852459054</v>
       </c>
       <c r="L20">
         <v>-2.766949164263762</v>
       </c>
       <c r="M20">
-        <v>-0.9076080541069285</v>
+        <v>-0.90760805410692846</v>
       </c>
       <c r="N20">
         <v>0.9355750020776552</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>-0.9413304377904532</v>
+        <v>-0.94133043779045322</v>
       </c>
       <c r="B21">
         <v>2.403180215591969</v>
       </c>
       <c r="C21">
-        <v>-0.1535311282080866</v>
+        <v>-0.15353112820808659</v>
       </c>
       <c r="D21">
         <v>0.8261364881200276</v>
@@ -1085,7 +1135,7 @@
         <v>1.123700025755241</v>
       </c>
       <c r="G21">
-        <v>-0.3051753742392728</v>
+        <v>-0.30517537423927282</v>
       </c>
       <c r="H21">
         <v>1.167793864196975</v>
@@ -1094,7 +1144,7 @@
         <v>1.416871143323146</v>
       </c>
       <c r="K21">
-        <v>-0.698807630381224</v>
+        <v>-0.69880763038122395</v>
       </c>
       <c r="L21">
         <v>-2.786496160377717</v>
@@ -1103,12 +1153,12 @@
         <v>-0.8863670467993765</v>
       </c>
       <c r="N21">
-        <v>0.9303152602000744</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
+        <v>0.93031526020007438</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>-0.9527111060884744</v>
+        <v>-0.95271110608847442</v>
       </c>
       <c r="B22">
         <v>2.436328078290781</v>
@@ -1117,7 +1167,7 @@
         <v>-0.1040466329721748</v>
       </c>
       <c r="D22">
-        <v>0.8123724534257072</v>
+        <v>0.81237245342570719</v>
       </c>
       <c r="F22">
         <v>1.089038755545648</v>
@@ -1132,121 +1182,121 @@
         <v>1.463966435568653</v>
       </c>
       <c r="K22">
-        <v>-0.7007675624244695</v>
+        <v>-0.70076756242446947</v>
       </c>
       <c r="L22">
-        <v>-2.80507363741543</v>
+        <v>-2.8050736374154299</v>
       </c>
       <c r="M22">
-        <v>-0.8651650808782959</v>
+        <v>-0.86516508087829591</v>
       </c>
       <c r="N22">
-        <v>0.9254075719582978</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
+        <v>0.92540757195829781</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>-0.9629152537866155</v>
+        <v>-0.96291525378661547</v>
       </c>
       <c r="B23">
         <v>2.466196001129167</v>
       </c>
       <c r="C23">
-        <v>-0.05542686612190764</v>
+        <v>-5.5426866121907642E-2</v>
       </c>
       <c r="D23">
-        <v>0.8001419873071234</v>
+        <v>0.80014198730712338</v>
       </c>
       <c r="F23">
         <v>1.053929347023886</v>
       </c>
       <c r="G23">
-        <v>-0.2873313126375628</v>
+        <v>-0.28733131263756279</v>
       </c>
       <c r="H23">
-        <v>1.140180535071107</v>
+        <v>1.1401805350711069</v>
       </c>
       <c r="I23">
         <v>1.514879342710574</v>
       </c>
       <c r="K23">
-        <v>-0.7024914263974287</v>
+        <v>-0.70249142639742868</v>
       </c>
       <c r="L23">
-        <v>-2.822704080673854</v>
+        <v>-2.8227040806738541</v>
       </c>
       <c r="M23">
-        <v>-0.8440031977504172</v>
+        <v>-0.84400319775041721</v>
       </c>
       <c r="N23">
-        <v>0.9208339495600056</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
+        <v>0.92083394956000564</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>-0.9719823971343229</v>
+        <v>-0.97198239713432288</v>
       </c>
       <c r="B24">
         <v>2.492903910573343</v>
       </c>
       <c r="C24">
-        <v>-0.007635253721223642</v>
+        <v>-7.6352537212236423E-3</v>
       </c>
       <c r="D24">
-        <v>0.7892875406527619</v>
+        <v>0.78928754065276185</v>
       </c>
       <c r="F24">
-        <v>1.01845600069441</v>
+        <v>1.0184560006944099</v>
       </c>
       <c r="G24">
-        <v>-0.2778790052273701</v>
+        <v>-0.27787900522737008</v>
       </c>
       <c r="H24">
-        <v>1.12418077421739</v>
+        <v>1.1241807742173899</v>
       </c>
       <c r="I24">
         <v>1.569931428115372</v>
       </c>
       <c r="K24">
-        <v>-0.703988279588069</v>
+        <v>-0.70398827958806898</v>
       </c>
       <c r="L24">
         <v>-2.839417841668328</v>
       </c>
       <c r="M24">
-        <v>-0.822871072865111</v>
+        <v>-0.82287107286511096</v>
       </c>
       <c r="N24">
-        <v>0.9165754996832556</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
+        <v>0.91657549968325558</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>-0.9799536556161532</v>
+        <v>-0.97995365561615322</v>
       </c>
       <c r="B25">
-        <v>2.516578445480526</v>
+        <v>2.5165784454805258</v>
       </c>
       <c r="C25">
-        <v>0.03937447454370659</v>
+        <v>3.9374474543706593E-2</v>
       </c>
       <c r="D25">
         <v>0.7796712163915952</v>
       </c>
       <c r="F25">
-        <v>0.9827447753727446</v>
+        <v>0.98274477537274463</v>
       </c>
       <c r="G25">
-        <v>-0.2680639217769811</v>
+        <v>-0.26806392177698107</v>
       </c>
       <c r="H25">
-        <v>1.106576380832431</v>
+        <v>1.1065763808324309</v>
       </c>
       <c r="I25">
         <v>1.629410157277309</v>
       </c>
       <c r="K25">
-        <v>-0.7052656003012192</v>
+        <v>-0.70526560030121921</v>
       </c>
       <c r="L25">
         <v>-2.855233630530833</v>
@@ -1258,7 +1308,7 @@
         <v>0.9126173984928404</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>-0.9868679389760654</v>
       </c>
@@ -1266,39 +1316,39 @@
         <v>2.537336808820108</v>
       </c>
       <c r="C26">
-        <v>0.08564104303343754</v>
+        <v>8.5641043033437544E-2</v>
       </c>
       <c r="D26">
-        <v>0.7711765009288784</v>
+        <v>0.77117650092887835</v>
       </c>
       <c r="F26">
-        <v>0.9469354966140641</v>
+        <v>0.94693549661406407</v>
       </c>
       <c r="G26">
         <v>-0.2578960949574356</v>
       </c>
       <c r="H26">
-        <v>1.087269230318681</v>
+        <v>1.0872692303186811</v>
       </c>
       <c r="I26">
-        <v>1.69358920035949</v>
+        <v>1.6935892003594899</v>
       </c>
       <c r="K26">
-        <v>-0.706331019060348</v>
+        <v>-0.70633101906034801</v>
       </c>
       <c r="L26">
         <v>-2.870170529810312</v>
       </c>
       <c r="M26">
-        <v>-0.7807120571509837</v>
+        <v>-0.78071205715098368</v>
       </c>
       <c r="N26">
-        <v>0.9089456067875816</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14">
+        <v>0.90894560678758163</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>-0.9927639646822825</v>
+        <v>-0.99276396468228245</v>
       </c>
       <c r="B27">
         <v>2.555297897619083</v>
@@ -1307,39 +1357,39 @@
         <v>0.1312203594111335</v>
       </c>
       <c r="D27">
-        <v>0.7637004550058581</v>
+        <v>0.76370045500585815</v>
       </c>
       <c r="F27">
-        <v>0.9023833319683804</v>
+        <v>0.90238333196838039</v>
       </c>
       <c r="G27">
-        <v>-0.2447620850359908</v>
+        <v>-0.24476208503599081</v>
       </c>
       <c r="H27">
-        <v>1.060683378233651</v>
+        <v>1.0606833782336511</v>
       </c>
       <c r="I27">
-        <v>1.780565268860753</v>
+        <v>1.7805652688607529</v>
       </c>
       <c r="K27">
-        <v>-0.7071920086784309</v>
+        <v>-0.70719200867843091</v>
       </c>
       <c r="L27">
-        <v>-2.884247719291627</v>
+        <v>-2.8842477192916269</v>
       </c>
       <c r="M27">
-        <v>-0.7596918368699264</v>
+        <v>-0.75969183686992636</v>
       </c>
       <c r="N27">
-        <v>0.9055469283435305</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14">
+        <v>0.90554692834353046</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>-0.9976696814389683</v>
+        <v>-0.99766968143896828</v>
       </c>
       <c r="B28">
-        <v>2.570542909648614</v>
+        <v>2.5705429096486139</v>
       </c>
       <c r="C28">
         <v>0.176083691573653</v>
@@ -1348,259 +1398,259 @@
         <v>0.757167117850569</v>
       </c>
       <c r="F28">
-        <v>0.8584617439968394</v>
+        <v>0.85846174399683939</v>
       </c>
       <c r="G28">
-        <v>-0.2312669748176482</v>
+        <v>-0.23126697481764821</v>
       </c>
       <c r="H28">
-        <v>1.031375517262708</v>
+        <v>1.0313755172627079</v>
       </c>
       <c r="I28">
         <v>1.87511490218328</v>
       </c>
       <c r="K28">
-        <v>-0.7078561002493549</v>
+        <v>-0.70785610024935486</v>
       </c>
       <c r="L28">
-        <v>-2.89748426197656</v>
+        <v>-2.8974842619765599</v>
       </c>
       <c r="M28">
         <v>-0.738716111428949</v>
       </c>
       <c r="N28">
-        <v>0.9024089245913962</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14">
+        <v>0.90240892459139621</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>-1.001620696773705</v>
+        <v>-1.0016206967737049</v>
       </c>
       <c r="B29">
         <v>2.583177305664488</v>
       </c>
       <c r="C29">
-        <v>0.2202900823634482</v>
+        <v>0.22029008236344819</v>
       </c>
       <c r="D29">
-        <v>0.7514989961202687</v>
+        <v>0.75149899612026871</v>
       </c>
       <c r="F29">
-        <v>0.8156720558476069</v>
+        <v>0.81567205584760694</v>
       </c>
       <c r="G29">
         <v>-0.2175720702245979</v>
       </c>
       <c r="H29">
-        <v>0.9995572278300922</v>
+        <v>0.99955722783009215</v>
       </c>
       <c r="I29">
-        <v>1.976921904043705</v>
+        <v>1.9769219040437049</v>
       </c>
       <c r="K29">
-        <v>-0.7083301752344541</v>
+        <v>-0.70833017523445407</v>
       </c>
       <c r="L29">
-        <v>-2.909909357482059</v>
+        <v>-2.9099093574820589</v>
       </c>
       <c r="M29">
         <v>-0.717767434858542</v>
       </c>
       <c r="N29">
-        <v>0.8995175150858017</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14">
+        <v>0.89951751508580169</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>-1.004642685872621</v>
       </c>
       <c r="B30">
-        <v>2.593276743093509</v>
+        <v>2.5932767430935089</v>
       </c>
       <c r="C30">
         <v>0.2638111855070252</v>
       </c>
       <c r="D30">
-        <v>0.746639437890769</v>
+        <v>0.74663943789076903</v>
       </c>
       <c r="F30">
         <v>0.7744561422076508</v>
       </c>
       <c r="G30">
-        <v>-0.2038911716691283</v>
+        <v>-0.20389117166912829</v>
       </c>
       <c r="H30">
-        <v>0.9656358470091648</v>
+        <v>0.96563584700916483</v>
       </c>
       <c r="I30">
-        <v>2.085446616240774</v>
+        <v>2.0854466162407741</v>
       </c>
       <c r="K30">
-        <v>-0.7086206919637552</v>
+        <v>-0.70862069196375521</v>
       </c>
       <c r="L30">
-        <v>-2.921535617347345</v>
+        <v>-2.9215356173473448</v>
       </c>
       <c r="M30">
-        <v>-0.6968572947850428</v>
+        <v>-0.69685729478504277</v>
       </c>
       <c r="N30">
-        <v>0.8968630277304246</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14">
+        <v>0.89686302773042459</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>-1.006764582571486</v>
+        <v>-1.0067645825714859</v>
       </c>
       <c r="B31">
         <v>2.600926858653728</v>
       </c>
       <c r="C31">
-        <v>0.3066992843684342</v>
+        <v>0.30669928436843419</v>
       </c>
       <c r="D31">
-        <v>0.742531821046639</v>
+        <v>0.74253182104663895</v>
       </c>
       <c r="F31">
-        <v>0.7351553513013867</v>
+        <v>0.73515535130138665</v>
       </c>
       <c r="G31">
-        <v>-0.1904211524478515</v>
+        <v>-0.19042115244785149</v>
       </c>
       <c r="H31">
-        <v>0.9302312139491316</v>
+        <v>0.93023121394913155</v>
       </c>
       <c r="I31">
-        <v>2.200028803367544</v>
+        <v>2.2000288033675441</v>
       </c>
       <c r="K31">
-        <v>-0.7087339100418337</v>
+        <v>-0.70873391004183373</v>
       </c>
       <c r="L31">
-        <v>-2.932379600882202</v>
+        <v>-2.9323796008822018</v>
       </c>
       <c r="M31">
-        <v>-0.6759902538424158</v>
+        <v>-0.67599025384241584</v>
       </c>
       <c r="N31">
-        <v>0.8944354172888865</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14">
+        <v>0.89443541728888654</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>-1.008009972124658</v>
       </c>
       <c r="B32">
-        <v>2.606191798231731</v>
+        <v>2.6061917982317309</v>
       </c>
       <c r="C32">
-        <v>0.3488569387967607</v>
+        <v>0.34885693879676072</v>
       </c>
       <c r="D32">
-        <v>0.7391384334465818</v>
+        <v>0.73913843344658181</v>
       </c>
       <c r="F32">
-        <v>0.6978857112758334</v>
+        <v>0.69788571127583343</v>
       </c>
       <c r="G32">
         <v>-0.1773900158855054</v>
       </c>
       <c r="H32">
-        <v>0.8940006605583005</v>
+        <v>0.89400066055830052</v>
       </c>
       <c r="I32">
-        <v>2.320330662292671</v>
+        <v>2.3203306622926712</v>
       </c>
       <c r="K32">
-        <v>-0.708675660541137</v>
+        <v>-0.70867566054113695</v>
       </c>
       <c r="L32">
-        <v>-2.942461101659179</v>
+        <v>-2.9424611016591791</v>
       </c>
       <c r="M32">
-        <v>-0.6551616572894166</v>
+        <v>-0.65516165728941655</v>
       </c>
       <c r="N32">
-        <v>0.892224434078924</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14">
+        <v>0.89222443407892404</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>-1.008402941859811</v>
+        <v>-1.0084029418598111</v>
       </c>
       <c r="B33">
         <v>2.60914892084981</v>
       </c>
       <c r="C33">
-        <v>0.3904424568958282</v>
+        <v>0.39044245689582818</v>
       </c>
       <c r="D33">
-        <v>0.736410372600699</v>
+        <v>0.73641037260069897</v>
       </c>
       <c r="F33">
-        <v>0.6627710848698909</v>
+        <v>0.66277108486989089</v>
       </c>
       <c r="G33">
-        <v>-0.1650150819911801</v>
+        <v>-0.16501508199118009</v>
       </c>
       <c r="H33">
         <v>0.8577579490216114</v>
       </c>
       <c r="I33">
-        <v>2.445770351766949</v>
+        <v>2.4457703517669489</v>
       </c>
       <c r="K33">
-        <v>-0.7084519411237983</v>
+        <v>-0.70845194112379828</v>
       </c>
       <c r="L33">
-        <v>-2.95179427070311</v>
+        <v>-2.9517942707031102</v>
       </c>
       <c r="M33">
-        <v>-0.6343806229174777</v>
+        <v>-0.63438062291747765</v>
       </c>
       <c r="N33">
-        <v>0.8902214022792854</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14">
+        <v>0.89022140227928537</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>-1.007955303481847</v>
+        <v>-1.0079553034818469</v>
       </c>
       <c r="B34">
-        <v>2.609834867916714</v>
+        <v>2.6098348679167138</v>
       </c>
       <c r="C34">
-        <v>0.4314447411220174</v>
+        <v>0.43144474112201742</v>
       </c>
       <c r="D34">
-        <v>0.7343222436210953</v>
+        <v>0.73432224362109533</v>
       </c>
       <c r="F34">
-        <v>0.6359889334485949</v>
+        <v>0.63598893344859486</v>
       </c>
       <c r="G34">
-        <v>-0.1556303596105648</v>
+        <v>-0.15563035961056479</v>
       </c>
       <c r="H34">
-        <v>0.8289546113667589</v>
+        <v>0.82895461136675885</v>
       </c>
       <c r="I34">
-        <v>2.550560407153758</v>
+        <v>2.5505604071537582</v>
       </c>
       <c r="K34">
-        <v>-0.7080680607046285</v>
+        <v>-0.70806806070462847</v>
       </c>
       <c r="L34">
-        <v>-2.960397022881175</v>
+        <v>-2.9603970228811751</v>
       </c>
       <c r="M34">
-        <v>-0.6136441891266582</v>
+        <v>-0.61364418912665819</v>
       </c>
       <c r="N34">
-        <v>0.8884175523593018</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14">
+        <v>0.88841755235930175</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>-1.007241584869915</v>
       </c>
@@ -1608,42 +1658,42 @@
         <v>2.609116489891222</v>
       </c>
       <c r="C35">
-        <v>0.4572635981158598</v>
+        <v>0.45726359811585982</v>
       </c>
       <c r="D35">
-        <v>0.7333155795726122</v>
+        <v>0.73331557957261218</v>
       </c>
       <c r="K35">
-        <v>-0.7075294260099653</v>
+        <v>-0.70752942600996527</v>
       </c>
       <c r="L35">
-        <v>-2.968287906689627</v>
+        <v>-2.9682879066896271</v>
       </c>
       <c r="M35">
-        <v>-0.5929492576766414</v>
+        <v>-0.59294925767664142</v>
       </c>
       <c r="N35">
-        <v>0.8868040005858895</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14">
+        <v>0.88680400058588948</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>-1.006211592958776</v>
       </c>
       <c r="B36">
-        <v>2.607540398960656</v>
+        <v>2.6075403989606558</v>
       </c>
       <c r="C36">
-        <v>0.482704720762835</v>
+        <v>0.48270472076283499</v>
       </c>
       <c r="D36">
-        <v>0.7325496186161876</v>
+        <v>0.73254961861618761</v>
       </c>
       <c r="K36">
-        <v>-0.7068418872672819</v>
+        <v>-0.70684188726728192</v>
       </c>
       <c r="L36">
-        <v>-2.975479636081886</v>
+        <v>-2.9754796360818858</v>
       </c>
       <c r="M36">
         <v>-0.5723093880244845</v>
@@ -1652,21 +1702,21 @@
         <v>0.8853735177300639</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>-1.004833096328578</v>
+        <v>-1.0048330963285781</v>
       </c>
       <c r="B37">
-        <v>2.605033146494783</v>
+        <v>2.6050331464947831</v>
       </c>
       <c r="C37">
-        <v>0.5080594725970538</v>
+        <v>0.50805947259705375</v>
       </c>
       <c r="D37">
-        <v>0.7320289638112716</v>
+        <v>0.73202896381127158</v>
       </c>
       <c r="K37">
-        <v>-0.7060089537438097</v>
+        <v>-0.70600895374380968</v>
       </c>
       <c r="L37">
         <v>-2.981992026409118</v>
@@ -1675,148 +1725,148 @@
         <v>-0.5517058143338881</v>
       </c>
       <c r="N37">
-        <v>0.884117618725445</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14">
+        <v>0.88411761872544503</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>-1.00313871834025</v>
       </c>
       <c r="B38">
-        <v>2.601671402902246</v>
+        <v>2.6016714029022459</v>
       </c>
       <c r="C38">
-        <v>0.5330542412008926</v>
+        <v>0.53305424120089262</v>
       </c>
       <c r="D38">
-        <v>0.7317446340375583</v>
+        <v>0.73174463403755829</v>
       </c>
       <c r="K38">
-        <v>-0.7050363383217079</v>
+        <v>-0.70503633832170787</v>
       </c>
       <c r="L38">
-        <v>-2.987833920104673</v>
+        <v>-2.9878339201046731</v>
       </c>
       <c r="M38">
-        <v>-0.5311608578839622</v>
+        <v>-0.53116085788396217</v>
       </c>
       <c r="N38">
         <v>0.8830305698364761</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>-1.001117696154819</v>
+        <v>-1.0011176961548189</v>
       </c>
       <c r="B39">
-        <v>2.597434644713142</v>
+        <v>2.5974346447131418</v>
       </c>
       <c r="C39">
-        <v>0.557849573817398</v>
+        <v>0.55784957381739797</v>
       </c>
       <c r="D39">
-        <v>0.7316930464259063</v>
+        <v>0.73169304642590627</v>
       </c>
       <c r="K39">
-        <v>-0.7039240562768038</v>
+        <v>-0.70392405627680377</v>
       </c>
       <c r="L39">
-        <v>-2.993025782551544</v>
+        <v>-2.9930257825515438</v>
       </c>
       <c r="M39">
-        <v>-0.5106267439890633</v>
+        <v>-0.51062674398906327</v>
       </c>
       <c r="N39">
-        <v>0.8821041019163589</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14">
+        <v>0.88210410191635891</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>-0.998779260601681</v>
+        <v>-0.99877926060168098</v>
       </c>
       <c r="B40">
-        <v>2.592345380346624</v>
+        <v>2.5923453803466239</v>
       </c>
       <c r="C40">
-        <v>0.5823685079196632</v>
+        <v>0.58236850791966321</v>
       </c>
       <c r="D40">
-        <v>0.7318710242965561</v>
+        <v>0.73187102429655615</v>
       </c>
       <c r="K40">
-        <v>-0.7026838836707847</v>
+        <v>-0.70268388367078471</v>
       </c>
       <c r="L40">
-        <v>-2.99756735711003</v>
+        <v>-2.9975673571100301</v>
       </c>
       <c r="M40">
-        <v>-0.490197053466589</v>
+        <v>-0.49019705346658898</v>
       </c>
       <c r="N40">
-        <v>0.8813345763297903</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14">
+        <v>0.88133457632979029</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>-0.9961312897830017</v>
+        <v>-0.99613128978300169</v>
       </c>
       <c r="B41">
-        <v>2.586424395532886</v>
+        <v>2.5864243955328861</v>
       </c>
       <c r="C41">
-        <v>0.6065806718590206</v>
+        <v>0.60658067185902065</v>
       </c>
       <c r="D41">
-        <v>0.7322742966580287</v>
+        <v>0.73227429665802868</v>
       </c>
       <c r="K41">
-        <v>-0.701315506808913</v>
+        <v>-0.70131550680891297</v>
       </c>
       <c r="L41">
         <v>-3.001485981684723</v>
       </c>
       <c r="M41">
-        <v>-0.4698066691419001</v>
+        <v>-0.46980666914190011</v>
       </c>
       <c r="N41">
-        <v>0.8807127073221543</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14">
+        <v>0.88071270732215434</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>-0.9931710418076998</v>
+        <v>-0.99317104180769977</v>
       </c>
       <c r="B42">
-        <v>2.579667455209101</v>
+        <v>2.5796674552091008</v>
       </c>
       <c r="C42">
         <v>0.6305293091880726</v>
       </c>
       <c r="D42">
-        <v>0.7329016947562237</v>
+        <v>0.73290169475622369</v>
       </c>
       <c r="K42">
-        <v>-0.6998247299623619</v>
+        <v>-0.69982472996236189</v>
       </c>
       <c r="L42">
-        <v>-3.004788834336075</v>
+        <v>-3.0047888343360749</v>
       </c>
       <c r="M42">
-        <v>-0.4494863749899795</v>
+        <v>-0.44948637498997951</v>
       </c>
       <c r="N42">
-        <v>0.8802363853245511</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14">
+        <v>0.88023638532455106</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>-0.9899002841975124</v>
+        <v>-0.98990028419751241</v>
       </c>
       <c r="B43">
         <v>2.572080080443496</v>
       </c>
       <c r="C43">
-        <v>0.6542074744117696</v>
+        <v>0.65420747441176963</v>
       </c>
       <c r="D43">
         <v>0.7337522059506022</v>
@@ -1825,128 +1875,128 @@
         <v>-0.6991811869396829</v>
       </c>
       <c r="L43">
-        <v>-3.005974113886001</v>
+        <v>-3.0059741138860012</v>
       </c>
       <c r="M43">
-        <v>-0.4411804380843338</v>
+        <v>-0.44118043808433383</v>
       </c>
       <c r="N43">
-        <v>0.8800841318106968</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14">
+        <v>0.88008413181069678</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>-0.9853758787278399</v>
+        <v>-0.98537587872783994</v>
       </c>
       <c r="B44">
-        <v>2.56143147456264</v>
+        <v>2.5614314745626401</v>
       </c>
       <c r="C44">
-        <v>0.6834225502487209</v>
+        <v>0.68342255024872089</v>
       </c>
       <c r="D44">
-        <v>0.7351262108190864</v>
+        <v>0.73512621081908636</v>
       </c>
       <c r="K44">
-        <v>-0.6985140986316393</v>
+        <v>-0.69851409863163927</v>
       </c>
       <c r="L44">
-        <v>-3.007062503167307</v>
+        <v>-3.0070625031673068</v>
       </c>
       <c r="M44">
-        <v>-0.4328453339108221</v>
+        <v>-0.43284533391082208</v>
       </c>
       <c r="N44">
-        <v>0.8799528621188654</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14">
+        <v>0.87995286211886536</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>-0.980374735670401</v>
+        <v>-0.98037473567040101</v>
       </c>
       <c r="B45">
         <v>2.549509851490821</v>
       </c>
       <c r="C45">
-        <v>0.7121794215503386</v>
+        <v>0.71217942155033864</v>
       </c>
       <c r="D45">
-        <v>0.736846290934414</v>
+        <v>0.73684629093441401</v>
       </c>
       <c r="K45">
         <v>-0.6978276334638257</v>
       </c>
       <c r="L45">
-        <v>-3.008041558138668</v>
+        <v>-3.0080415581386681</v>
       </c>
       <c r="M45">
-        <v>-0.4245450073354438</v>
+        <v>-0.42454500733544381</v>
       </c>
       <c r="N45">
-        <v>0.879846211026787</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14">
+        <v>0.87984621102678695</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>-0.9749064804212595</v>
+        <v>-0.97490648042125949</v>
       </c>
       <c r="B46">
-        <v>2.536341450076442</v>
+        <v>2.5363414500764421</v>
       </c>
       <c r="C46">
-        <v>0.7404437912071165</v>
+        <v>0.74044379120711645</v>
       </c>
       <c r="D46">
         <v>0.7389100502413487</v>
       </c>
       <c r="K46">
-        <v>-0.6971220471155486</v>
+        <v>-0.69712204711554859</v>
       </c>
       <c r="L46">
-        <v>-3.00892203925011</v>
+        <v>-3.0089220392501099</v>
       </c>
       <c r="M46">
-        <v>-0.416257194904656</v>
+        <v>-0.41625719490465601</v>
       </c>
       <c r="N46">
-        <v>0.8797613777907697</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14">
+        <v>0.87976137779076968</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>-0.968962626339948</v>
+        <v>-0.96896262633994801</v>
       </c>
       <c r="B47">
-        <v>2.5219076338656</v>
+        <v>2.5219076338656001</v>
       </c>
       <c r="C47">
         <v>0.7682540385592439</v>
       </c>
       <c r="D47">
-        <v>0.7413234716915392</v>
+        <v>0.74132347169153923</v>
       </c>
       <c r="K47">
-        <v>-0.6963950156839132</v>
+        <v>-0.69639501568391315</v>
       </c>
       <c r="L47">
-        <v>-3.009702713145399</v>
+        <v>-3.0097027131453991</v>
       </c>
       <c r="M47">
-        <v>-0.4079640916001921</v>
+        <v>-0.40796409160019209</v>
       </c>
       <c r="N47">
-        <v>0.8796986361167488</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14">
+        <v>0.87969863611674881</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>-0.9625468268513543</v>
+        <v>-0.96254682685135429</v>
       </c>
       <c r="B48">
-        <v>2.506219258787395</v>
+        <v>2.5062192587873948</v>
       </c>
       <c r="C48">
-        <v>0.7955847688876482</v>
+        <v>0.79558476888764817</v>
       </c>
       <c r="D48">
         <v>0.7440891737076043</v>
@@ -1955,434 +2005,434 @@
         <v>-0.6956502192705859</v>
       </c>
       <c r="L48">
-        <v>-3.010385661008755</v>
+        <v>-3.0103856610087552</v>
       </c>
       <c r="M48">
-        <v>-0.3996933671523809</v>
+        <v>-0.39969336715238091</v>
       </c>
       <c r="N48">
         <v>0.8796570101162936</v>
       </c>
     </row>
-    <row r="49" spans="1:14">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>-0.9556559499939485</v>
+        <v>-0.95565594999394854</v>
       </c>
       <c r="B49">
-        <v>2.489270556532119</v>
+        <v>2.4892705565321189</v>
       </c>
       <c r="C49">
-        <v>0.8224363899254215</v>
+        <v>0.82243638992542145</v>
       </c>
       <c r="D49">
-        <v>0.7472132376133093</v>
+        <v>0.74721323761330927</v>
       </c>
       <c r="K49">
-        <v>-0.6948871933896998</v>
+        <v>-0.69488719338969984</v>
       </c>
       <c r="L49">
-        <v>-3.010972645908985</v>
+        <v>-3.0109726459089852</v>
       </c>
       <c r="M49">
-        <v>-0.3914368033116413</v>
+        <v>-0.39143680331164132</v>
       </c>
       <c r="N49">
-        <v>0.8796360945407762</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14">
+        <v>0.87963609454077618</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>-0.9463772855328667</v>
+        <v>-0.94637728553286671</v>
       </c>
       <c r="B50">
-        <v>2.466322579714005</v>
+        <v>2.4663225797140051</v>
       </c>
       <c r="C50">
-        <v>0.8552905726249758</v>
+        <v>0.85529057262497576</v>
       </c>
       <c r="D50">
-        <v>0.7516225163067495</v>
+        <v>0.75162251630674948</v>
       </c>
       <c r="K50">
-        <v>-0.6941053772916116</v>
+        <v>-0.69410537729161159</v>
       </c>
       <c r="L50">
         <v>-3.011464034538788</v>
       </c>
       <c r="M50">
-        <v>-0.3831884436301192</v>
+        <v>-0.38318844363011922</v>
       </c>
       <c r="N50">
-        <v>0.8796358337688006</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14">
+        <v>0.87963583376880061</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>-0.9337298834656872</v>
+        <v>-0.93372988346568719</v>
       </c>
       <c r="B51">
-        <v>2.434864457762975</v>
+        <v>2.4348644577629752</v>
       </c>
       <c r="C51">
-        <v>0.8952176750778362</v>
+        <v>0.89521767507783623</v>
       </c>
       <c r="D51">
-        <v>0.7579439663165722</v>
+        <v>0.75794396631657224</v>
       </c>
       <c r="K51">
-        <v>-0.693304409960279</v>
+        <v>-0.69330440996027898</v>
       </c>
       <c r="L51">
-        <v>-3.011860191385363</v>
+        <v>-3.0118601913853631</v>
       </c>
       <c r="M51">
-        <v>-0.3749440048473057</v>
+        <v>-0.37494400484730572</v>
       </c>
       <c r="N51">
-        <v>0.8796558509227014</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14">
+        <v>0.87965585092270138</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>-0.9199044746714784</v>
       </c>
       <c r="B52">
-        <v>2.400300442600616</v>
+        <v>2.4003004426006158</v>
       </c>
       <c r="C52">
-        <v>0.9338175833434895</v>
+        <v>0.93381758334348952</v>
       </c>
       <c r="D52">
         <v>0.7652136531727719</v>
       </c>
       <c r="K52">
-        <v>-0.692485274723166</v>
+        <v>-0.69248527472316601</v>
       </c>
       <c r="L52">
         <v>-3.012161861061549</v>
       </c>
       <c r="M52">
-        <v>-0.3667105384043455</v>
+        <v>-0.36671053840434548</v>
       </c>
       <c r="N52">
-        <v>0.8796955495427856</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14">
+        <v>0.87969554954278562</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>-0.9049091005180142</v>
+        <v>-0.90490910051801421</v>
       </c>
       <c r="B53">
-        <v>2.362658332193743</v>
+        <v>2.3626583321937429</v>
       </c>
       <c r="C53">
-        <v>0.9709662321609069</v>
+        <v>0.97096623216090694</v>
       </c>
       <c r="D53">
-        <v>0.7734659252306871</v>
+        <v>0.77346592523068713</v>
       </c>
       <c r="K53">
-        <v>-0.6916483103726183</v>
+        <v>-0.69164831037261831</v>
       </c>
       <c r="L53">
         <v>-3.012369583160122</v>
       </c>
       <c r="M53">
-        <v>-0.3584898137662134</v>
+        <v>-0.35848981376621342</v>
       </c>
       <c r="N53">
-        <v>0.8797547043978596</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14">
+        <v>0.87975470439785963</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>-0.8887011747073588</v>
+        <v>-0.88870117470735877</v>
       </c>
       <c r="B54">
-        <v>2.321838255143812</v>
+        <v>2.3218382551438119</v>
       </c>
       <c r="C54">
         <v>1.006631366545633</v>
       </c>
       <c r="D54">
-        <v>0.78276889280567</v>
+        <v>0.78276889280566997</v>
       </c>
       <c r="K54">
-        <v>-0.6907933819780379</v>
+        <v>-0.69079338197803786</v>
       </c>
       <c r="L54">
         <v>-3.012484017723545</v>
       </c>
       <c r="M54">
-        <v>-0.3502789795210088</v>
+        <v>-0.35027897952100878</v>
       </c>
       <c r="N54">
-        <v>0.8798331304668066</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14">
+        <v>0.87983313046680656</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>-0.8712628484163699</v>
+        <v>-0.87126284841636992</v>
       </c>
       <c r="B55">
-        <v>2.277802639087641</v>
+        <v>2.2778026390876409</v>
       </c>
       <c r="C55">
         <v>1.040694921899918</v>
       </c>
       <c r="D55">
-        <v>0.7931864464616307</v>
+        <v>0.79318644646163072</v>
       </c>
       <c r="K55">
-        <v>-0.689920876554583</v>
+        <v>-0.68992087655458301</v>
       </c>
       <c r="L55">
-        <v>-3.012506393045032</v>
+        <v>-3.0125063930450322</v>
       </c>
       <c r="M55">
-        <v>-0.3420786687434033</v>
+        <v>-0.34207866874340331</v>
       </c>
       <c r="N55">
-        <v>0.8799302447448858</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14">
+        <v>0.87993024474488579</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>-0.8525631300952851</v>
+        <v>-0.85256313009528506</v>
       </c>
       <c r="B56">
-        <v>2.230480881255229</v>
+        <v>2.2304808812552288</v>
       </c>
       <c r="C56">
-        <v>1.073041610857984</v>
+        <v>1.0730416108579841</v>
       </c>
       <c r="D56">
-        <v>0.804797323619208</v>
+        <v>0.80479732361920797</v>
       </c>
       <c r="K56">
-        <v>-0.6890310327594711</v>
+        <v>-0.68903103275947108</v>
       </c>
       <c r="L56">
-        <v>-3.012437241818755</v>
+        <v>-3.0124372418187551</v>
       </c>
       <c r="M56">
-        <v>-0.3338897790803403</v>
+        <v>-0.33388977908034029</v>
       </c>
       <c r="N56">
-        <v>0.8800458817613668</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14">
+        <v>0.88004588176136678</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>-0.832558444180477</v>
+        <v>-0.83255844418047698</v>
       </c>
       <c r="B57">
-        <v>2.179771082539626</v>
+        <v>2.1797710825396259</v>
       </c>
       <c r="C57">
-        <v>1.103540270393997</v>
+        <v>1.1035402703939969</v>
       </c>
       <c r="D57">
-        <v>0.8176983144957304</v>
+        <v>0.81769831449573038</v>
       </c>
       <c r="K57">
-        <v>-0.6881239025070663</v>
+        <v>-0.68812390250706634</v>
       </c>
       <c r="L57">
-        <v>-3.012277426275055</v>
+        <v>-3.0122774262750549</v>
       </c>
       <c r="M57">
-        <v>-0.3257105745064193</v>
+        <v>-0.32571057450641933</v>
       </c>
       <c r="N57">
-        <v>0.8801795497909901</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14">
+        <v>0.88017954979099011</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>-0.8112049614667712</v>
+        <v>-0.81120496146677123</v>
       </c>
       <c r="B58">
-        <v>2.125570952525229</v>
+        <v>2.1255709525252291</v>
       </c>
       <c r="C58">
         <v>1.132026831288518</v>
       </c>
       <c r="D58">
-        <v>0.831995930957305</v>
+        <v>0.83199593095730495</v>
       </c>
       <c r="K58">
-        <v>-0.6871996665009831</v>
+        <v>-0.68719966650098308</v>
       </c>
       <c r="L58">
-        <v>-3.012027264737151</v>
+        <v>-3.0120272647371511</v>
       </c>
       <c r="M58">
         <v>-0.3175419471827739</v>
       </c>
       <c r="N58">
-        <v>0.8803309680673749</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14">
+        <v>0.88033096806737487</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>-0.7884584163367147</v>
+        <v>-0.78845841633671465</v>
       </c>
       <c r="B59">
-        <v>2.067777609701973</v>
+        <v>2.0677776097019729</v>
       </c>
       <c r="C59">
-        <v>1.158304498054204</v>
+        <v>1.1583044980542041</v>
       </c>
       <c r="D59">
-        <v>0.8478104209008729</v>
+        <v>0.84781042090087289</v>
       </c>
       <c r="K59">
-        <v>-0.6862583413831401</v>
+        <v>-0.68625834138314012</v>
       </c>
       <c r="L59">
-        <v>-3.011687082366587</v>
+        <v>-3.0116870823665871</v>
       </c>
       <c r="M59">
-        <v>-0.3093831959777038</v>
+        <v>-0.30938319597770381</v>
       </c>
       <c r="N59">
         <v>0.8804998469202836</v>
       </c>
     </row>
-    <row r="60" spans="1:14">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>-0.7643076465804726</v>
+        <v>-0.76430764658047257</v>
       </c>
       <c r="B60">
-        <v>2.006373518594175</v>
+        <v>2.0063735185941751</v>
       </c>
       <c r="C60">
         <v>1.182118399979164</v>
       </c>
       <c r="D60">
-        <v>0.8652516737569806</v>
+        <v>0.86525167375698064</v>
       </c>
       <c r="K60">
-        <v>-0.6850579913739192</v>
+        <v>-0.68505799137391921</v>
       </c>
       <c r="L60">
-        <v>-3.011136190269392</v>
+        <v>-3.0111361902693918</v>
       </c>
       <c r="M60">
-        <v>-0.2991994942923946</v>
+        <v>-0.29919949429239462</v>
       </c>
       <c r="N60">
-        <v>0.8807337348725613</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14">
+        <v>0.88073373487256135</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>-0.7387138350225966</v>
+        <v>-0.73871383502259658</v>
       </c>
       <c r="B61">
         <v>1.941272889362194</v>
       </c>
       <c r="C61">
-        <v>1.203210633833362</v>
+        <v>1.2032106338333619</v>
       </c>
       <c r="D61">
-        <v>0.8844645482503972</v>
+        <v>0.88446454825039722</v>
       </c>
       <c r="K61">
-        <v>-0.6838321779179523</v>
+        <v>-0.68383217791795226</v>
       </c>
       <c r="L61">
-        <v>-3.010447827558219</v>
+        <v>-3.0104478275582189</v>
       </c>
       <c r="M61">
-        <v>-0.2890351925000912</v>
+        <v>-0.28903519250009119</v>
       </c>
       <c r="N61">
-        <v>0.880993569072016</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14">
+        <v>0.88099356907201598</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>-0.7115584104496306</v>
+        <v>-0.71155841044963064</v>
       </c>
       <c r="B62">
-        <v>1.872187185214209</v>
+        <v>1.8721871852142089</v>
       </c>
       <c r="C62">
-        <v>1.221317016660414</v>
+        <v>1.2213170166604139</v>
       </c>
       <c r="D62">
-        <v>0.9056809375189896</v>
+        <v>0.90568093751898959</v>
       </c>
       <c r="K62">
-        <v>-0.6822634990763076</v>
+        <v>-0.68226349907630757</v>
       </c>
       <c r="L62">
-        <v>-3.009394337083952</v>
+        <v>-3.0093943370839522</v>
       </c>
       <c r="M62">
-        <v>-0.2763504049734165</v>
+        <v>-0.27635040497341651</v>
       </c>
       <c r="N62">
-        <v>0.8813519756295847</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14">
+        <v>0.88135197562958467</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>-0.6827974509389775</v>
+        <v>-0.68279745093897748</v>
       </c>
       <c r="B63">
-        <v>1.799017540897946</v>
+        <v>1.7990175408979461</v>
       </c>
       <c r="C63">
         <v>1.236066319428603</v>
       </c>
       <c r="D63">
-        <v>0.9290128332855704</v>
+        <v>0.92901283328557038</v>
       </c>
       <c r="K63">
-        <v>-0.6806555799278924</v>
+        <v>-0.68065557992789238</v>
       </c>
       <c r="L63">
-        <v>-3.00812921771742</v>
+        <v>-3.0081292177174199</v>
       </c>
       <c r="M63">
-        <v>-0.2636935157495396</v>
+        <v>-0.26369351574953959</v>
       </c>
       <c r="N63">
-        <v>0.8817486639372935</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14">
+        <v>0.88174866393729345</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>-0.6524556926031406</v>
+        <v>-0.65245569260314062</v>
       </c>
       <c r="B64">
-        <v>1.721845213210203</v>
+        <v>1.7218452132102029</v>
       </c>
       <c r="C64">
         <v>1.247005355542834</v>
       </c>
       <c r="D64">
-        <v>0.9546128004035332</v>
+        <v>0.95461280040353325</v>
       </c>
       <c r="K64">
-        <v>-0.6790086864613729</v>
+        <v>-0.67900868646137291</v>
       </c>
       <c r="L64">
-        <v>-3.006654011453496</v>
+        <v>-3.0066540114534961</v>
       </c>
       <c r="M64">
-        <v>-0.2510628959009151</v>
+        <v>-0.25106289590091507</v>
       </c>
       <c r="N64">
-        <v>0.882182394469361</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14">
+        <v>0.88218239446936098</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>-0.6205248240410752</v>
+        <v>-0.62052482404107523</v>
       </c>
       <c r="B65">
         <v>1.640668258423184</v>
@@ -2391,88 +2441,88 @@
         <v>1.253680042251109</v>
       </c>
       <c r="D65">
-        <v>0.982548846154876</v>
+        <v>0.98254884615487603</v>
       </c>
       <c r="K65">
-        <v>-0.677324702357756</v>
+        <v>-0.67732470235775599</v>
       </c>
       <c r="L65">
-        <v>-3.004973036476941</v>
+        <v>-3.0049730364769411</v>
       </c>
       <c r="M65">
-        <v>-0.2384665079726755</v>
+        <v>-0.23846650797267549</v>
       </c>
       <c r="N65">
-        <v>0.8826517238898017</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14">
+        <v>0.88265172388980173</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>-0.5871118326283141</v>
+        <v>-0.58711183262831412</v>
       </c>
       <c r="B66">
-        <v>1.5557798932176</v>
+        <v>1.5557798932175999</v>
       </c>
       <c r="C66">
         <v>1.255576227298481</v>
       </c>
       <c r="D66">
-        <v>1.012579099976124</v>
+        <v>1.0125790999761239</v>
       </c>
       <c r="K66">
-        <v>-0.6751658319213208</v>
+        <v>-0.67516583192132085</v>
       </c>
       <c r="L66">
-        <v>-3.002581675476307</v>
+        <v>-3.0025816754763071</v>
       </c>
       <c r="M66">
-        <v>-0.2227536154766382</v>
+        <v>-0.22275361547663819</v>
       </c>
       <c r="N66">
-        <v>0.8832836065707769</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14">
+        <v>0.88328360657077687</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>-0.5526298803570341</v>
+        <v>-0.55262988035703409</v>
       </c>
       <c r="B67">
-        <v>1.468254740157318</v>
+        <v>1.4682547401573181</v>
       </c>
       <c r="C67">
-        <v>1.252254423245229</v>
+        <v>1.2522544232452291</v>
       </c>
       <c r="D67">
-        <v>1.044526129132577</v>
+        <v>1.0445261291325769</v>
       </c>
       <c r="K67">
-        <v>-0.6723857531673554</v>
+        <v>-0.67238575316735538</v>
       </c>
       <c r="L67">
-        <v>-2.999146718289693</v>
+        <v>-2.9991467182896931</v>
       </c>
       <c r="M67">
-        <v>-0.2031721400645942</v>
+        <v>-0.20317214006459419</v>
       </c>
       <c r="N67">
-        <v>0.8841389069683468</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14">
+        <v>0.88413890696834685</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>-0.5171699238316279</v>
+        <v>-0.51716992383162785</v>
       </c>
       <c r="B68">
-        <v>1.378347595430966</v>
+        <v>1.3783475954309661</v>
       </c>
       <c r="C68">
-        <v>1.243331471098921</v>
+        <v>1.2433314710989209</v>
       </c>
       <c r="D68">
-        <v>1.078346079867747</v>
+        <v>1.0783460798677471</v>
       </c>
       <c r="K68">
-        <v>-0.669516574098373</v>
+        <v>-0.66951657409837295</v>
       </c>
       <c r="L68">
         <v>-2.995221765112233</v>
@@ -2484,9 +2534,9 @@
         <v>0.885069358054411</v>
       </c>
     </row>
-    <row r="69" spans="1:14">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>-0.488017262097959</v>
+        <v>-0.48801726209795898</v>
       </c>
       <c r="B69">
         <v>1.304520363721515</v>
@@ -2498,53 +2548,53 @@
         <v>1.108105301714112</v>
       </c>
       <c r="K69">
-        <v>-0.6665611679722173</v>
+        <v>-0.66656116797221732</v>
       </c>
       <c r="L69">
-        <v>-2.99081579161606</v>
+        <v>-2.9908157916160598</v>
       </c>
       <c r="M69">
-        <v>-0.164219715586477</v>
+        <v>-0.16421971558647699</v>
       </c>
       <c r="N69">
-        <v>0.8860696582928048</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14">
+        <v>0.88606965829280482</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>-0.4583654830963486</v>
+        <v>-0.45836548309634861</v>
       </c>
       <c r="B70">
-        <v>1.229526180393519</v>
+        <v>1.2295261803935189</v>
       </c>
       <c r="C70">
-        <v>1.216125820180428</v>
+        <v>1.2161258201804279</v>
       </c>
       <c r="D70">
-        <v>1.137515245179315</v>
+        <v>1.1375152451793149</v>
       </c>
       <c r="K70">
-        <v>-0.6635219886073372</v>
+        <v>-0.66352198860733724</v>
       </c>
       <c r="L70">
-        <v>-2.985937418523782</v>
+        <v>-2.9859374185237821</v>
       </c>
       <c r="M70">
-        <v>-0.1448597619337114</v>
+        <v>-0.14485976193371139</v>
       </c>
       <c r="N70">
-        <v>0.8871352784174276</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14">
+        <v>0.88713527841742756</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>-0.4292552345809895</v>
+        <v>-0.42925523458098952</v>
       </c>
       <c r="B71">
         <v>1.156010438332131</v>
       </c>
       <c r="C71">
-        <v>1.196859866792496</v>
+        <v>1.1968598667924959</v>
       </c>
       <c r="D71">
         <v>1.165667970159368</v>
@@ -2553,18 +2603,18 @@
         <v>-0.6603979350784609</v>
       </c>
       <c r="L71">
-        <v>-2.980587522255023</v>
+        <v>-2.9805875222550231</v>
       </c>
       <c r="M71">
-        <v>-0.1255649841949132</v>
+        <v>-0.12556498419491319</v>
       </c>
       <c r="N71">
-        <v>0.8882614726933576</v>
-      </c>
-    </row>
-    <row r="72" spans="1:14">
+        <v>0.88826147269335765</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>-0.4008588700544661</v>
+        <v>-0.40085887005446608</v>
       </c>
       <c r="B72">
         <v>1.084416574664997</v>
@@ -2576,24 +2626,24 @@
         <v>1.186232073378459</v>
       </c>
       <c r="K72">
-        <v>-0.6571922135947051</v>
+        <v>-0.65719221359470514</v>
       </c>
       <c r="L72">
-        <v>-2.974775154322482</v>
+        <v>-2.9747751543224821</v>
       </c>
       <c r="M72">
         <v>-0.1063470814263951</v>
       </c>
       <c r="N72">
-        <v>0.8894427068597814</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14">
+        <v>0.88944270685978144</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>-0.3743080969578209</v>
+        <v>-0.37430809695782091</v>
       </c>
       <c r="B73">
-        <v>1.017596548285355</v>
+        <v>1.0175965482853551</v>
       </c>
       <c r="C73">
         <v>1.149537548898464</v>
@@ -2602,102 +2652,102 @@
         <v>1.197960964661732</v>
       </c>
       <c r="K73">
-        <v>-0.6530730184521881</v>
+        <v>-0.65307301845218813</v>
       </c>
       <c r="L73">
-        <v>-2.966869927559087</v>
+        <v>-2.9668699275590869</v>
       </c>
       <c r="M73">
-        <v>-0.08243638681401526</v>
+        <v>-8.2436386814015258E-2</v>
       </c>
       <c r="N73">
-        <v>0.8909756890078666</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14">
+        <v>0.89097568900786661</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>-0.3493302805462291</v>
+        <v>-0.34933028054622911</v>
       </c>
       <c r="B74">
-        <v>0.9548559453496012</v>
+        <v>0.95485594534960117</v>
       </c>
       <c r="C74">
-        <v>1.123006002321476</v>
+        <v>1.1230060023214761</v>
       </c>
       <c r="D74">
-        <v>1.194808196097498</v>
+        <v>1.1948081960974981</v>
       </c>
       <c r="K74">
-        <v>-0.6488273653809041</v>
+        <v>-0.64882736538090413</v>
       </c>
       <c r="L74">
-        <v>-2.958253177011739</v>
+        <v>-2.9582531770117391</v>
       </c>
       <c r="M74">
-        <v>-0.05863197027695772</v>
+        <v>-5.8631970276957719E-2</v>
       </c>
       <c r="N74">
-        <v>0.8925748924663767</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14">
+        <v>0.89257489246637667</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>-0.3265723696523103</v>
+        <v>-0.32657236965231029</v>
       </c>
       <c r="B75">
-        <v>0.8978099679244371</v>
+        <v>0.89780996792443712</v>
       </c>
       <c r="C75">
         <v>1.095948202494947</v>
       </c>
       <c r="D75">
-        <v>1.183692032469088</v>
+        <v>1.1836920324690881</v>
       </c>
       <c r="K75">
-        <v>-0.644463436163227</v>
+        <v>-0.64446343616322699</v>
       </c>
       <c r="L75">
         <v>-2.948947094135407</v>
       </c>
       <c r="M75">
-        <v>-0.03496509059075784</v>
+        <v>-3.4965090590757843E-2</v>
       </c>
       <c r="N75">
-        <v>0.8942299053982257</v>
-      </c>
-    </row>
-    <row r="76" spans="1:14">
+        <v>0.89422990539822567</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>-0.3091279509390075</v>
+        <v>-0.30912795093900752</v>
       </c>
       <c r="B76">
-        <v>0.8541671694996883</v>
+        <v>0.85416716949968829</v>
       </c>
       <c r="C76">
         <v>1.073215176444027</v>
       </c>
       <c r="D76">
-        <v>1.152773352339089</v>
+        <v>1.1527733523390891</v>
       </c>
       <c r="K76">
         <v>-0.6399784099270267</v>
       </c>
       <c r="L76">
-        <v>-2.938948920131348</v>
+        <v>-2.9389489201313479</v>
       </c>
       <c r="M76">
-        <v>-0.0114142607209464</v>
+        <v>-1.1414260720946401E-2</v>
       </c>
       <c r="N76">
-        <v>0.8959291402940531</v>
-      </c>
-    </row>
-    <row r="77" spans="1:14">
+        <v>0.89592914029405313</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>-0.2932131439233731</v>
+        <v>-0.29321314392337311</v>
       </c>
       <c r="B77">
-        <v>0.8144228507885425</v>
+        <v>0.81442285078854249</v>
       </c>
       <c r="C77">
         <v>1.050899028571525</v>
@@ -2706,24 +2756,24 @@
         <v>1.085799658788817</v>
       </c>
       <c r="K77">
-        <v>-0.6353752770892581</v>
+        <v>-0.63537527708925812</v>
       </c>
       <c r="L77">
-        <v>-2.928268055519549</v>
+        <v>-2.9282680555195491</v>
       </c>
       <c r="M77">
-        <v>0.01201051282813276</v>
+        <v>1.201051282813276E-2</v>
       </c>
       <c r="N77">
-        <v>0.8976602246962117</v>
-      </c>
-    </row>
-    <row r="78" spans="1:14">
+        <v>0.89766022469621165</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>-0.2790646060836996</v>
       </c>
       <c r="B78">
-        <v>0.7791534010959655</v>
+        <v>0.77915340109596554</v>
       </c>
       <c r="C78">
         <v>1.029748139617694</v>
@@ -2732,102 +2782,102 @@
         <v>1.042810481894759</v>
       </c>
       <c r="K78">
-        <v>-0.6306599311681804</v>
+        <v>-0.63065993116818042</v>
       </c>
       <c r="L78">
-        <v>-2.916922663930136</v>
+        <v>-2.9169226639301362</v>
       </c>
       <c r="M78">
-        <v>0.03529039463774422</v>
+        <v>3.5290394637744221E-2</v>
       </c>
       <c r="N78">
-        <v>0.8994110834270287</v>
-      </c>
-    </row>
-    <row r="79" spans="1:14">
+        <v>0.89941108342702869</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>-0.2643006372331755</v>
+        <v>-0.26430063723317548</v>
       </c>
       <c r="B79">
-        <v>0.742418920276219</v>
+        <v>0.74241892027621903</v>
       </c>
       <c r="C79">
         <v>1.006279184067878</v>
       </c>
       <c r="D79">
-        <v>0.9525281107921472</v>
+        <v>0.95252811079214716</v>
       </c>
       <c r="K79">
-        <v>-0.6258309391241735</v>
+        <v>-0.62583093912417354</v>
       </c>
       <c r="L79">
-        <v>-2.904911712032184</v>
+        <v>-2.9049117120321841</v>
       </c>
       <c r="M79">
-        <v>0.05843631722545346</v>
+        <v>5.8436317225453463E-2</v>
       </c>
       <c r="N79">
-        <v>0.901171085011198</v>
-      </c>
-    </row>
-    <row r="80" spans="1:14">
+        <v>0.90117108501119803</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>-0.2510061223975615</v>
+        <v>-0.25100612239756148</v>
       </c>
       <c r="B80">
-        <v>0.7094079465142858</v>
+        <v>0.70940794651428585</v>
       </c>
       <c r="C80">
-        <v>0.9838629485196512</v>
+        <v>0.98386294851965117</v>
       </c>
       <c r="D80">
-        <v>0.8903307020333294</v>
+        <v>0.89033070203332942</v>
       </c>
       <c r="K80">
-        <v>-0.6208854488259172</v>
+        <v>-0.62088544882591723</v>
       </c>
       <c r="L80">
-        <v>-2.892227879903764</v>
+        <v>-2.8922278799037642</v>
       </c>
       <c r="M80">
-        <v>0.08146161971127829</v>
+        <v>8.1461619711278285E-2</v>
       </c>
       <c r="N80">
-        <v>0.902926715031397</v>
-      </c>
-    </row>
-    <row r="81" spans="1:14">
+        <v>0.90292671503139699</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>-0.2372165107983654</v>
+        <v>-0.23721651079836539</v>
       </c>
       <c r="B81">
-        <v>0.6752427306237143</v>
+        <v>0.67524273062371432</v>
       </c>
       <c r="C81">
-        <v>0.9592698255676054</v>
+        <v>0.95926982556760543</v>
       </c>
       <c r="D81">
-        <v>0.7939772123465098</v>
+        <v>0.79397721234650975</v>
       </c>
       <c r="K81">
-        <v>-0.615826741801376</v>
+        <v>-0.61582674180137598</v>
       </c>
       <c r="L81">
-        <v>-2.878880699856094</v>
+        <v>-2.8788806998560941</v>
       </c>
       <c r="M81">
-        <v>0.1043528484346875</v>
+        <v>0.10435284843468751</v>
       </c>
       <c r="N81">
-        <v>0.9046592219446176</v>
-      </c>
-    </row>
-    <row r="82" spans="1:14">
+        <v>0.90465922194461756</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>-0.224306374199844</v>
+        <v>-0.22430637419984401</v>
       </c>
       <c r="B82">
-        <v>0.6433325837586376</v>
+        <v>0.64333258375863756</v>
       </c>
       <c r="C82">
         <v>0.9349191820739422</v>
@@ -2836,127 +2886,127 @@
         <v>0.5729145202278727</v>
       </c>
       <c r="K82">
-        <v>-0.609346521583424</v>
+        <v>-0.60934652158342395</v>
       </c>
       <c r="L82">
-        <v>-2.861270904113878</v>
+        <v>-2.8612709041138782</v>
       </c>
       <c r="M82">
         <v>0.1327667618297014</v>
       </c>
       <c r="N82">
-        <v>0.9067305070770544</v>
-      </c>
-    </row>
-    <row r="83" spans="1:14">
+        <v>0.90673050707705438</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>-0.2138869063344795</v>
+        <v>-0.21388690633447949</v>
       </c>
       <c r="B83">
         <v>0.6176391548212804</v>
       </c>
       <c r="C83">
-        <v>0.9142807336508736</v>
+        <v>0.91428073365087359</v>
       </c>
       <c r="D83">
-        <v>0.4493807342861281</v>
+        <v>0.44938073428612813</v>
       </c>
       <c r="K83">
-        <v>-0.6026967787255484</v>
+        <v>-0.60269677872554839</v>
       </c>
       <c r="L83">
-        <v>-2.842647581622509</v>
+        <v>-2.8426475816225092</v>
       </c>
       <c r="M83">
-        <v>0.1609417148633255</v>
+        <v>0.16094171486332551</v>
       </c>
       <c r="N83">
-        <v>0.9087105614594324</v>
-      </c>
-    </row>
-    <row r="84" spans="1:14">
+        <v>0.90871056145943241</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>-0.2031794322868365</v>
+        <v>-0.20317943228683649</v>
       </c>
       <c r="B84">
-        <v>0.591298239144314</v>
+        <v>0.59129823914431401</v>
       </c>
       <c r="C84">
-        <v>0.8920998444677721</v>
+        <v>0.89209984446777213</v>
       </c>
       <c r="D84">
-        <v>0.2700574833297076</v>
+        <v>0.27005748332970758</v>
       </c>
       <c r="K84">
-        <v>-0.5958726598842703</v>
+        <v>-0.59587265988427029</v>
       </c>
       <c r="L84">
-        <v>-2.822995888827738</v>
+        <v>-2.8229958888277382</v>
       </c>
       <c r="M84">
         <v>0.1888932815410197</v>
       </c>
       <c r="N84">
-        <v>0.9105556248982128</v>
-      </c>
-    </row>
-    <row r="85" spans="1:14">
+        <v>0.91055562489821285</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>-0.1940020213588003</v>
+        <v>-0.19400202135880029</v>
       </c>
       <c r="B85">
-        <v>0.5689157476891588</v>
+        <v>0.56891574768915876</v>
       </c>
       <c r="C85">
-        <v>0.8723710776291276</v>
+        <v>0.87237107762912758</v>
       </c>
       <c r="D85">
-        <v>0.185984517952918</v>
+        <v>0.18598451795291801</v>
       </c>
       <c r="K85">
-        <v>-0.5871000018742538</v>
+        <v>-0.58710000187425382</v>
       </c>
       <c r="L85">
-        <v>-2.796990584442964</v>
+        <v>-2.7969905844429639</v>
       </c>
       <c r="M85">
-        <v>0.2234930626973891</v>
+        <v>0.22349306269738911</v>
       </c>
       <c r="N85">
-        <v>0.9125263817302161</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14">
+        <v>0.91252638173021605</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="K86">
-        <v>-0.5780648051007267</v>
+        <v>-0.57806480510072666</v>
       </c>
       <c r="L86">
-        <v>-2.769401486042607</v>
+        <v>-2.7694014860426068</v>
       </c>
       <c r="M86">
-        <v>0.2576801232070484</v>
+        <v>0.25768012320704842</v>
       </c>
       <c r="N86">
         <v>0.914132097982714</v>
       </c>
     </row>
-    <row r="87" spans="1:14">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="K87">
-        <v>-0.5687608861588795</v>
+        <v>-0.56876088615887954</v>
       </c>
       <c r="L87">
-        <v>-2.740204409404009</v>
+        <v>-2.7402044094040088</v>
       </c>
       <c r="M87">
-        <v>0.2914570425325378</v>
+        <v>0.29145704253253779</v>
       </c>
       <c r="N87">
-        <v>0.9152730189969328</v>
-      </c>
-    </row>
-    <row r="88" spans="1:14">
+        <v>0.91527301899693281</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="K88">
-        <v>-0.5567536513496472</v>
+        <v>-0.55675365134964716</v>
       </c>
       <c r="L88">
         <v>-2.701438711801134</v>
@@ -2965,166 +3015,166 @@
         <v>0.3330586951947288</v>
       </c>
       <c r="N88">
-        <v>0.9156846113118836</v>
-      </c>
-    </row>
-    <row r="89" spans="1:14">
+        <v>0.91568461131188361</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="K89">
-        <v>-0.5443323823580347</v>
+        <v>-0.54433238235803472</v>
       </c>
       <c r="L89">
         <v>-2.660152999174195</v>
       </c>
       <c r="M89">
-        <v>0.3739020190179217</v>
+        <v>0.37390201901792169</v>
       </c>
       <c r="N89">
-        <v>0.9149221804801476</v>
-      </c>
-    </row>
-    <row r="90" spans="1:14">
+        <v>0.91492218048014762</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="K90">
-        <v>-0.5314771037670114</v>
+        <v>-0.53147710376701141</v>
       </c>
       <c r="L90">
-        <v>-2.61625494147363</v>
+        <v>-2.6162549414736298</v>
       </c>
       <c r="M90">
-        <v>0.4139760948963919</v>
+        <v>0.41397609489639192</v>
       </c>
       <c r="N90">
-        <v>0.9126850537093024</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14">
+        <v>0.91268505370930242</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="K91">
-        <v>-0.5181864823719662</v>
+        <v>-0.51818648237196618</v>
       </c>
       <c r="L91">
-        <v>-2.569713167170528</v>
+        <v>-2.5697131671705278</v>
       </c>
       <c r="M91">
-        <v>0.4531986496427255</v>
+        <v>0.45319864964272549</v>
       </c>
       <c r="N91">
-        <v>0.9086502246136184</v>
-      </c>
-    </row>
-    <row r="92" spans="1:14">
+        <v>0.90865022461361844</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="K92">
         <v>-0.5044454509029862</v>
       </c>
       <c r="L92">
-        <v>-2.520443890236077</v>
+        <v>-2.5204438902360771</v>
       </c>
       <c r="M92">
-        <v>0.4915097819969225</v>
+        <v>0.49150978199692252</v>
       </c>
       <c r="N92">
-        <v>0.902472042356178</v>
-      </c>
-    </row>
-    <row r="93" spans="1:14">
+        <v>0.90247204235617795</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="K93">
-        <v>-0.4902334243876471</v>
+        <v>-0.49023342438764711</v>
       </c>
       <c r="L93">
-        <v>-2.468330224810601</v>
+        <v>-2.4683302248106012</v>
       </c>
       <c r="M93">
-        <v>0.5288481612692428</v>
+        <v>0.52884816126924283</v>
       </c>
       <c r="N93">
-        <v>0.8935476065774405</v>
-      </c>
-    </row>
-    <row r="94" spans="1:14">
+        <v>0.89354760657744048</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="K94">
-        <v>-0.4757181330179491</v>
+        <v>-0.47571813301794907</v>
       </c>
       <c r="L94">
         <v>-2.413306437442825</v>
       </c>
       <c r="M94">
-        <v>0.5650777249694001</v>
+        <v>0.56507772496940012</v>
       </c>
       <c r="N94">
-        <v>0.8814030149762712</v>
-      </c>
-    </row>
-    <row r="95" spans="1:14">
+        <v>0.88140301497627116</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="K95">
-        <v>-0.4605482674961393</v>
+        <v>-0.46054826749613931</v>
       </c>
       <c r="L95">
-        <v>-2.355317697954023</v>
+        <v>-2.3553176979540229</v>
       </c>
       <c r="M95">
-        <v>0.6000723590613022</v>
+        <v>0.60007235906130219</v>
       </c>
       <c r="N95">
-        <v>0.8653269484582441</v>
-      </c>
-    </row>
-    <row r="96" spans="1:14">
+        <v>0.86532694845824409</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="K96">
-        <v>-0.4448985165509979</v>
+        <v>-0.44489851655099788</v>
       </c>
       <c r="L96">
         <v>-2.294302069534949</v>
       </c>
       <c r="M96">
-        <v>0.6336663409002082</v>
+        <v>0.63366634090020824</v>
       </c>
       <c r="N96">
-        <v>0.8450104472578804</v>
-      </c>
-    </row>
-    <row r="97" spans="11:14">
+        <v>0.84501044725788044</v>
+      </c>
+    </row>
+    <row r="97" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K97">
-        <v>-0.4287405602801984</v>
+        <v>-0.42874056028019841</v>
       </c>
       <c r="L97">
-        <v>-2.230088756007992</v>
+        <v>-2.2300887560079921</v>
       </c>
       <c r="M97">
-        <v>0.6657417356924418</v>
+        <v>0.66574173569244177</v>
       </c>
       <c r="N97">
-        <v>0.8203283124517451</v>
-      </c>
-    </row>
-    <row r="98" spans="11:14">
+        <v>0.82032831245174509</v>
+      </c>
+    </row>
+    <row r="98" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K98">
-        <v>-0.4119665249286253</v>
+        <v>-0.41196652492862529</v>
       </c>
       <c r="L98">
-        <v>-2.16216145691454</v>
+        <v>-2.1621614569145402</v>
       </c>
       <c r="M98">
         <v>0.6962632750471518</v>
       </c>
       <c r="N98">
-        <v>0.7896448257792575</v>
-      </c>
-    </row>
-    <row r="99" spans="11:14">
+        <v>0.78964482577925754</v>
+      </c>
+    </row>
+    <row r="99" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K99">
-        <v>-0.3946278791160517</v>
+        <v>-0.39462787911605168</v>
       </c>
       <c r="L99">
-        <v>-2.090638022171315</v>
+        <v>-2.0906380221713148</v>
       </c>
       <c r="M99">
-        <v>0.7248638273751318</v>
+        <v>0.72486382737513178</v>
       </c>
       <c r="N99">
-        <v>0.7505205998188231</v>
-      </c>
-    </row>
-    <row r="100" spans="11:14">
+        <v>0.75052059981882313</v>
+      </c>
+    </row>
+    <row r="100" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K100">
-        <v>-0.3768777391748208</v>
+        <v>-0.37687773917482081</v>
       </c>
       <c r="L100">
         <v>-2.016076334231145</v>
@@ -3136,357 +3186,357 @@
         <v>0.7039404063795266</v>
       </c>
     </row>
-    <row r="101" spans="11:14">
+    <row r="101" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K101">
-        <v>-0.358642058785837</v>
+        <v>-0.35864205878583699</v>
       </c>
       <c r="L101">
         <v>-1.938096842953148</v>
       </c>
       <c r="M101">
-        <v>0.7746978539189375</v>
+        <v>0.77469785391893753</v>
       </c>
       <c r="N101">
-        <v>0.6502871705123573</v>
-      </c>
-    </row>
-    <row r="102" spans="11:14">
+        <v>0.65028717051235729</v>
+      </c>
+    </row>
+    <row r="102" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K102">
-        <v>-0.33988069867378</v>
+        <v>-0.33988069867378001</v>
       </c>
       <c r="L102">
-        <v>-1.85643571141584</v>
+        <v>-1.8564357114158401</v>
       </c>
       <c r="M102">
         <v>0.7955298069063893</v>
       </c>
       <c r="N102">
-        <v>0.5891665983902746</v>
-      </c>
-    </row>
-    <row r="103" spans="11:14">
+        <v>0.58916659839027463</v>
+      </c>
+    </row>
+    <row r="103" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K103">
-        <v>-0.3206887082197133</v>
+        <v>-0.32068870821971329</v>
       </c>
       <c r="L103">
-        <v>-1.771421535583137</v>
+        <v>-1.7714215355831371</v>
       </c>
       <c r="M103">
-        <v>0.8131174925682845</v>
+        <v>0.81311749256828447</v>
       </c>
       <c r="N103">
-        <v>0.522133434859145</v>
-      </c>
-    </row>
-    <row r="104" spans="11:14">
+        <v>0.52213343485914498</v>
+      </c>
+    </row>
+    <row r="104" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K104">
-        <v>-0.3011361893009069</v>
+        <v>-0.30113618930090691</v>
       </c>
       <c r="L104">
-        <v>-1.683290099313257</v>
+        <v>-1.6832900993132569</v>
       </c>
       <c r="M104">
-        <v>0.8270697720843216</v>
+        <v>0.82706977208432164</v>
       </c>
       <c r="N104">
-        <v>0.4412306039636161</v>
-      </c>
-    </row>
-    <row r="105" spans="11:14">
+        <v>0.44123060396361607</v>
+      </c>
+    </row>
+    <row r="105" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K105">
-        <v>-0.2818585745483403</v>
+        <v>-0.28185857454834029</v>
       </c>
       <c r="L105">
-        <v>-1.594905802155204</v>
+        <v>-1.5949058021552041</v>
       </c>
       <c r="M105">
-        <v>0.8367742878985751</v>
+        <v>0.83677428789857511</v>
       </c>
       <c r="N105">
-        <v>0.3582418316384867</v>
-      </c>
-    </row>
-    <row r="106" spans="11:14">
+        <v>0.35824183163848672</v>
+      </c>
+    </row>
+    <row r="106" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K106">
-        <v>-0.2627062994330586</v>
+        <v>-0.26270629943305862</v>
       </c>
       <c r="L106">
-        <v>-1.505637913134536</v>
+        <v>-1.5056379131345361</v>
       </c>
       <c r="M106">
-        <v>0.8422634177865866</v>
+        <v>0.84226341778658664</v>
       </c>
       <c r="N106">
-        <v>0.2684445967403619</v>
-      </c>
-    </row>
-    <row r="107" spans="11:14">
+        <v>0.26844459674036192</v>
+      </c>
+    </row>
+    <row r="107" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K107">
-        <v>-0.2443869669213173</v>
+        <v>-0.24438696692131731</v>
       </c>
       <c r="L107">
-        <v>-1.418907530607244</v>
+        <v>-1.4189075306072441</v>
       </c>
       <c r="M107">
-        <v>0.8434724247277089</v>
+        <v>0.84347242472770889</v>
       </c>
       <c r="N107">
-        <v>0.1753237368342075</v>
-      </c>
-    </row>
-    <row r="108" spans="11:14">
+        <v>0.17532373683420749</v>
+      </c>
+    </row>
+    <row r="108" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K108">
-        <v>-0.2275005844316645</v>
+        <v>-0.22750058443166449</v>
       </c>
       <c r="L108">
-        <v>-1.33781033181854</v>
+        <v>-1.3378103318185399</v>
       </c>
       <c r="M108">
-        <v>0.8409031954128015</v>
+        <v>0.84090319541280145</v>
       </c>
       <c r="N108">
         <v>0.1040867939601901</v>
       </c>
     </row>
-    <row r="109" spans="11:14">
+    <row r="109" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K109">
-        <v>-0.2115534816234683</v>
+        <v>-0.21155348162346829</v>
       </c>
       <c r="L109">
-        <v>-1.260225901113161</v>
+        <v>-1.2602259011131609</v>
       </c>
       <c r="M109">
-        <v>0.835042440872017</v>
+        <v>0.83504244087201696</v>
       </c>
       <c r="N109">
-        <v>0.06469795910563655</v>
-      </c>
-    </row>
-    <row r="110" spans="11:14">
+        <v>6.4697959105636554E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K110">
         <v>-0.1985921513138966</v>
       </c>
       <c r="L110">
-        <v>-1.19646541722677</v>
+        <v>-1.1964654172267699</v>
       </c>
       <c r="M110">
-        <v>0.8276692620039675</v>
+        <v>0.82766926200396751</v>
       </c>
       <c r="N110">
-        <v>0.03376394492347554</v>
-      </c>
-    </row>
-    <row r="111" spans="11:14">
+        <v>3.3763944923475543E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K111">
-        <v>-0.1870389713219326</v>
+        <v>-0.18703897132193259</v>
       </c>
       <c r="L111">
-        <v>-1.139126337535295</v>
+        <v>-1.1391263375352949</v>
       </c>
       <c r="M111">
-        <v>0.8190301863481854</v>
+        <v>0.81903018634818536</v>
       </c>
       <c r="N111">
-        <v>0.0105019457659612</v>
-      </c>
-    </row>
-    <row r="112" spans="11:14">
+        <v>1.0501945765961199E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K112">
-        <v>-0.1772036216107135</v>
+        <v>-0.17720362161071351</v>
       </c>
       <c r="L112">
-        <v>-1.089957099638934</v>
+        <v>-1.0899570996389341</v>
       </c>
       <c r="M112">
-        <v>0.8100724636668296</v>
+        <v>0.81007246366682961</v>
       </c>
       <c r="N112">
-        <v>0.002753988681648458</v>
-      </c>
-    </row>
-    <row r="113" spans="11:14">
+        <v>2.7539886816484579E-3</v>
+      </c>
+    </row>
+    <row r="113" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K113">
-        <v>-0.1680297942070925</v>
+        <v>-0.16802979420709249</v>
       </c>
       <c r="L113">
         <v>-1.043823158571493</v>
       </c>
       <c r="M113">
-        <v>0.8003419691032549</v>
+        <v>0.80034196910325495</v>
       </c>
       <c r="N113">
-        <v>0.0001884817813486499</v>
-      </c>
-    </row>
-    <row r="114" spans="11:14">
+        <v>1.884817813486499E-4</v>
+      </c>
+    </row>
+    <row r="114" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K114">
         <v>-0.160317349776714</v>
       </c>
       <c r="L114">
-        <v>-1.004846705652718</v>
+        <v>-1.0048467056527179</v>
       </c>
       <c r="M114">
-        <v>0.7910839976115347</v>
+        <v>0.79108399761153469</v>
       </c>
       <c r="N114">
         <v>1.800032633802929E-11</v>
       </c>
     </row>
-    <row r="115" spans="11:14">
+    <row r="115" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K115">
         <v>-0.1579278673868576</v>
       </c>
       <c r="L115">
-        <v>-0.9927386690832308</v>
+        <v>-0.99273866908323083</v>
       </c>
       <c r="M115">
-        <v>0.7880125935762071</v>
+        <v>0.78801259357620712</v>
       </c>
       <c r="N115">
-        <v>2.079218639172772E-12</v>
-      </c>
-    </row>
-    <row r="116" spans="11:14">
+        <v>2.0792186391727722E-12</v>
+      </c>
+    </row>
+    <row r="116" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K116">
-        <v>-0.1549657890175659</v>
+        <v>-0.15496578901756591</v>
       </c>
       <c r="L116">
-        <v>-0.977709539671764</v>
+        <v>-0.97770953967176399</v>
       </c>
       <c r="M116">
-        <v>0.7840694486671682</v>
+        <v>0.78406944866716821</v>
       </c>
       <c r="N116">
-        <v>5.778199250894747E-13</v>
-      </c>
-    </row>
-    <row r="117" spans="11:14">
+        <v>5.7781992508947466E-13</v>
+      </c>
+    </row>
+    <row r="117" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K117">
         <v>-0.1513890618832256</v>
       </c>
       <c r="L117">
-        <v>-0.9595340404055868</v>
+        <v>-0.95953404040558676</v>
       </c>
       <c r="M117">
-        <v>0.7791048672602398</v>
+        <v>0.77910486726023975</v>
       </c>
       <c r="N117">
         <v>1.010492489492617E-13</v>
       </c>
     </row>
-    <row r="118" spans="11:14">
+    <row r="118" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K118">
         <v>-0.147891708569409</v>
       </c>
       <c r="L118">
-        <v>-0.9417343952543522</v>
+        <v>-0.94173439525435221</v>
       </c>
       <c r="M118">
-        <v>0.7740321281950432</v>
+        <v>0.77403212819504319</v>
       </c>
       <c r="N118">
-        <v>4.236114137891397E-14</v>
-      </c>
-    </row>
-    <row r="119" spans="11:14">
+        <v>4.2361141378913967E-14</v>
+      </c>
+    </row>
+    <row r="119" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K119">
-        <v>-0.1437306287431794</v>
+        <v>-0.14373062874317941</v>
       </c>
       <c r="L119">
-        <v>-0.9205248523371471</v>
+        <v>-0.92052485233714709</v>
       </c>
       <c r="M119">
-        <v>0.7677117181806907</v>
+        <v>0.76771171818069073</v>
       </c>
       <c r="N119">
-        <v>1.197258102851314E-17</v>
-      </c>
-    </row>
-    <row r="120" spans="11:14">
+        <v>1.1972581028513141E-17</v>
+      </c>
+    </row>
+    <row r="120" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K120">
-        <v>-0.1412301667528416</v>
+        <v>-0.14123016675284161</v>
       </c>
       <c r="L120">
-        <v>-0.9077650202889928</v>
+        <v>-0.90776502028899275</v>
       </c>
       <c r="M120">
-        <v>0.7637634632562126</v>
+        <v>0.76376346325621258</v>
       </c>
       <c r="N120">
-        <v>2.041315549354512E-18</v>
-      </c>
-    </row>
-    <row r="121" spans="11:14">
+        <v>2.0413155493545119E-18</v>
+      </c>
+    </row>
+    <row r="121" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K121">
-        <v>-0.1379769279609392</v>
+        <v>-0.13797692796093919</v>
       </c>
       <c r="L121">
-        <v>-0.8911484849644163</v>
+        <v>-0.89114848496441634</v>
       </c>
       <c r="M121">
-        <v>0.7584542936899731</v>
+        <v>0.75845429368997308</v>
       </c>
       <c r="N121">
-        <v>1.154663731602855E-19</v>
-      </c>
-    </row>
-    <row r="122" spans="11:14">
+        <v>1.1546637316028549E-19</v>
+      </c>
+    </row>
+    <row r="122" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K122">
         <v>-0.1348781914528096</v>
       </c>
       <c r="L122">
-        <v>-0.875307380271874</v>
+        <v>-0.87530738027187405</v>
       </c>
       <c r="M122">
-        <v>0.7532146162064151</v>
+        <v>0.75321461620641506</v>
       </c>
       <c r="N122">
-        <v>3.13899388082915E-21</v>
-      </c>
-    </row>
-    <row r="123" spans="11:14">
+        <v>3.1389938808291499E-21</v>
+      </c>
+    </row>
+    <row r="123" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K123">
         <v>-0.1319731496891586</v>
       </c>
       <c r="L123">
-        <v>-0.8604466296118775</v>
+        <v>-0.86044662961187746</v>
       </c>
       <c r="M123">
-        <v>0.748139420991041</v>
+        <v>0.74813942099104103</v>
       </c>
       <c r="N123">
-        <v>8.995338238193286E-22</v>
-      </c>
-    </row>
-    <row r="124" spans="11:14">
+        <v>8.9953382381932858E-22</v>
+      </c>
+    </row>
+    <row r="124" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K124">
         <v>-0.128229432450402</v>
       </c>
       <c r="L124">
-        <v>-0.8412845331063831</v>
+        <v>-0.84128453310638307</v>
       </c>
       <c r="M124">
-        <v>0.7413630318647292</v>
+        <v>0.74136303186472918</v>
       </c>
       <c r="N124">
         <v>3.12328254931981E-22</v>
       </c>
     </row>
-    <row r="125" spans="11:14">
+    <row r="125" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K125">
         <v>-0.1240560322667677</v>
       </c>
       <c r="L125">
-        <v>-0.8199137661772656</v>
+        <v>-0.81991376617726563</v>
       </c>
       <c r="M125">
-        <v>0.7334925776094245</v>
+        <v>0.73349257760942455</v>
       </c>
       <c r="N125">
-        <v>1.422670977950533E-22</v>
-      </c>
-    </row>
-    <row r="126" spans="11:14">
+        <v>1.4226709779505329E-22</v>
+      </c>
+    </row>
+    <row r="126" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K126">
         <v>-0.1194177477730283</v>
       </c>
@@ -3494,21 +3544,21 @@
         <v>-0.7961582528100144</v>
       </c>
       <c r="M126">
-        <v>0.7243467738383269</v>
+        <v>0.72434677383832691</v>
       </c>
       <c r="N126">
         <v>1.039393416858965E-22</v>
       </c>
     </row>
-    <row r="127" spans="11:14">
+    <row r="127" spans="11:14" x14ac:dyDescent="0.2">
       <c r="K127">
         <v>-0.1147074776286346</v>
       </c>
       <c r="L127">
-        <v>-0.7720410985980923</v>
+        <v>-0.77204109859809233</v>
       </c>
       <c r="M127">
-        <v>0.7146271942498721</v>
+        <v>0.71462719424987209</v>
       </c>
       <c r="N127">
         <v>5.152204277831799E-23</v>

</xml_diff>